<commit_message>
0.0.b2.1.1 GUI Code Cleaned Up
</commit_message>
<xml_diff>
--- a/Roadmap.xlsx
+++ b/Roadmap.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17030"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
   <workbookPr showObjects="none" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16457" windowHeight="6720" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16457" windowHeight="6720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Roadmap" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="745">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="753">
   <si>
     <t>56 pixels</t>
   </si>
@@ -2271,6 +2271,30 @@
   </si>
   <si>
     <t>Save to a read only folder</t>
+  </si>
+  <si>
+    <t>0.0.a43</t>
+  </si>
+  <si>
+    <t>Update Documentation</t>
+  </si>
+  <si>
+    <t>0.1.a6</t>
+  </si>
+  <si>
+    <t>0.6.a5</t>
+  </si>
+  <si>
+    <t>0.5.a4</t>
+  </si>
+  <si>
+    <t>0.3.a9</t>
+  </si>
+  <si>
+    <t>0.4.a2.2</t>
+  </si>
+  <si>
+    <t>0.2.a7</t>
   </si>
 </sst>
 </file>
@@ -23897,10 +23921,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L100"/>
+  <dimension ref="A1:L107"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -23951,10 +23975,10 @@
       <c r="B3" t="s">
         <v>512</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="24" t="s">
         <v>513</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="24" t="s">
         <v>625</v>
       </c>
       <c r="I3" t="s">
@@ -24373,377 +24397,374 @@
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B46" s="5" t="s">
+      <c r="B46" t="s">
+        <v>745</v>
+      </c>
+      <c r="C46" t="s">
+        <v>652</v>
+      </c>
+      <c r="D46" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B47" s="5" t="s">
         <v>665</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>666</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D47" s="5" t="s">
         <v>682</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E47" s="5" t="s">
         <v>683</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B47" t="s">
-        <v>514</v>
-      </c>
-      <c r="C47" t="s">
-        <v>652</v>
-      </c>
-      <c r="D47" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B48" t="s">
-        <v>632</v>
+        <v>514</v>
       </c>
       <c r="C48" t="s">
-        <v>513</v>
+        <v>652</v>
       </c>
       <c r="D48" t="s">
-        <v>626</v>
-      </c>
-      <c r="E48" t="s">
-        <v>627</v>
+        <v>515</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B49" t="s">
-        <v>633</v>
+        <v>632</v>
+      </c>
+      <c r="C49" t="s">
+        <v>513</v>
+      </c>
+      <c r="D49" t="s">
+        <v>626</v>
       </c>
       <c r="E49" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B50" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E50" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B51" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="E51" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B52" t="s">
+        <v>635</v>
+      </c>
+      <c r="E52" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B53" t="s">
         <v>636</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E53" t="s">
         <v>631</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B53" s="5" t="s">
-        <v>667</v>
-      </c>
-      <c r="C53" t="s">
-        <v>666</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>682</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B54" t="s">
-        <v>526</v>
+        <v>747</v>
       </c>
       <c r="C54" t="s">
         <v>652</v>
       </c>
       <c r="D54" t="s">
-        <v>516</v>
+        <v>746</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B55" t="s">
-        <v>529</v>
-      </c>
-      <c r="D55" t="s">
-        <v>518</v>
+      <c r="B55" s="5" t="s">
+        <v>667</v>
+      </c>
+      <c r="C55" t="s">
+        <v>666</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>682</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>683</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B56" t="s">
-        <v>568</v>
+        <v>526</v>
+      </c>
+      <c r="C56" t="s">
+        <v>652</v>
       </c>
       <c r="D56" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B57" t="s">
-        <v>569</v>
+        <v>529</v>
       </c>
       <c r="D57" t="s">
-        <v>542</v>
+        <v>518</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B58" t="s">
-        <v>646</v>
-      </c>
-      <c r="C58" t="s">
-        <v>513</v>
+        <v>568</v>
       </c>
       <c r="D58" t="s">
-        <v>637</v>
-      </c>
-      <c r="E58" t="s">
-        <v>641</v>
+        <v>522</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B59" t="s">
-        <v>647</v>
-      </c>
-      <c r="E59" t="s">
-        <v>642</v>
+        <v>569</v>
+      </c>
+      <c r="D59" t="s">
+        <v>542</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B60" t="s">
-        <v>648</v>
+        <v>646</v>
+      </c>
+      <c r="C60" t="s">
+        <v>513</v>
       </c>
       <c r="D60" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="E60" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B61" t="s">
-        <v>649</v>
-      </c>
-      <c r="D61" t="s">
-        <v>639</v>
+        <v>647</v>
       </c>
       <c r="E61" t="s">
-        <v>111</v>
+        <v>642</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B62" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="D62" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="E62" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B63" t="s">
-        <v>651</v>
+        <v>649</v>
+      </c>
+      <c r="D63" t="s">
+        <v>639</v>
       </c>
       <c r="E63" t="s">
-        <v>645</v>
+        <v>111</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B64" s="5" t="s">
-        <v>668</v>
-      </c>
-      <c r="C64" t="s">
-        <v>666</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>682</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>683</v>
+      <c r="B64" t="s">
+        <v>650</v>
+      </c>
+      <c r="D64" t="s">
+        <v>640</v>
+      </c>
+      <c r="E64" t="s">
+        <v>644</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B65" t="s">
-        <v>530</v>
-      </c>
-      <c r="C65" t="s">
-        <v>652</v>
-      </c>
-      <c r="D65" t="s">
-        <v>548</v>
+        <v>651</v>
+      </c>
+      <c r="E65" t="s">
+        <v>645</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B66" t="s">
-        <v>570</v>
+        <v>752</v>
+      </c>
+      <c r="C66" t="s">
+        <v>652</v>
       </c>
       <c r="D66" t="s">
-        <v>517</v>
+        <v>746</v>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B67" t="s">
-        <v>653</v>
-      </c>
-      <c r="D67" t="s">
-        <v>657</v>
+      <c r="B67" s="5" t="s">
+        <v>668</v>
+      </c>
+      <c r="C67" t="s">
+        <v>666</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>682</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>683</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B68" t="s">
-        <v>654</v>
+        <v>530</v>
+      </c>
+      <c r="C68" t="s">
+        <v>652</v>
       </c>
       <c r="D68" t="s">
-        <v>567</v>
+        <v>548</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B69" t="s">
-        <v>740</v>
+        <v>570</v>
       </c>
       <c r="D69" t="s">
-        <v>741</v>
+        <v>517</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B70" t="s">
-        <v>549</v>
-      </c>
-      <c r="C70" t="s">
-        <v>513</v>
+        <v>653</v>
       </c>
       <c r="D70" t="s">
-        <v>655</v>
-      </c>
-      <c r="E70" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B71" t="s">
-        <v>550</v>
-      </c>
-      <c r="E71" t="s">
-        <v>660</v>
+        <v>654</v>
+      </c>
+      <c r="D71" t="s">
+        <v>567</v>
       </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B72" t="s">
-        <v>661</v>
+        <v>740</v>
       </c>
       <c r="D72" t="s">
-        <v>656</v>
-      </c>
-      <c r="E72" t="s">
-        <v>669</v>
+        <v>741</v>
       </c>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B73" t="s">
-        <v>662</v>
+        <v>549</v>
+      </c>
+      <c r="C73" t="s">
+        <v>513</v>
+      </c>
+      <c r="D73" t="s">
+        <v>655</v>
       </c>
       <c r="E73" t="s">
-        <v>670</v>
+        <v>659</v>
       </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B74" t="s">
-        <v>663</v>
-      </c>
-      <c r="D74" t="s">
-        <v>671</v>
+        <v>550</v>
       </c>
       <c r="E74" t="s">
-        <v>111</v>
+        <v>660</v>
       </c>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B75" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="D75" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="E75" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B76" t="s">
-        <v>674</v>
+        <v>662</v>
       </c>
       <c r="E76" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B77" t="s">
-        <v>742</v>
+        <v>663</v>
       </c>
       <c r="D77" t="s">
-        <v>743</v>
+        <v>671</v>
       </c>
       <c r="E77" t="s">
-        <v>744</v>
+        <v>111</v>
       </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B78" s="5" t="s">
-        <v>675</v>
-      </c>
-      <c r="C78" t="s">
-        <v>666</v>
-      </c>
-      <c r="D78" s="5" t="s">
-        <v>682</v>
-      </c>
-      <c r="E78" s="5" t="s">
-        <v>683</v>
+      <c r="B78" t="s">
+        <v>664</v>
+      </c>
+      <c r="D78" t="s">
+        <v>658</v>
+      </c>
+      <c r="E78" t="s">
+        <v>672</v>
       </c>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B79" t="s">
-        <v>531</v>
-      </c>
-      <c r="C79" t="s">
-        <v>652</v>
-      </c>
-      <c r="D79" t="s">
-        <v>519</v>
+        <v>674</v>
+      </c>
+      <c r="E79" t="s">
+        <v>673</v>
       </c>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B80" t="s">
-        <v>676</v>
+        <v>742</v>
       </c>
       <c r="D80" t="s">
-        <v>520</v>
+        <v>743</v>
+      </c>
+      <c r="E80" t="s">
+        <v>744</v>
       </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B81" t="s">
-        <v>533</v>
+        <v>750</v>
       </c>
       <c r="C81" t="s">
-        <v>513</v>
+        <v>652</v>
       </c>
       <c r="D81" t="s">
-        <v>677</v>
-      </c>
-      <c r="E81" t="s">
-        <v>679</v>
+        <v>746</v>
       </c>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B82" s="5" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="C82" t="s">
         <v>666</v>
@@ -24757,45 +24778,51 @@
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B83" t="s">
-        <v>680</v>
+        <v>531</v>
       </c>
       <c r="C83" t="s">
         <v>652</v>
       </c>
       <c r="D83" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B84" t="s">
-        <v>681</v>
+        <v>676</v>
       </c>
       <c r="D84" t="s">
-        <v>534</v>
-      </c>
-      <c r="E84" t="s">
-        <v>684</v>
+        <v>520</v>
       </c>
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B85" t="s">
-        <v>686</v>
+        <v>533</v>
+      </c>
+      <c r="C85" t="s">
+        <v>513</v>
+      </c>
+      <c r="D85" t="s">
+        <v>677</v>
       </c>
       <c r="E85" t="s">
-        <v>559</v>
+        <v>679</v>
       </c>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B86" t="s">
-        <v>687</v>
-      </c>
-      <c r="E86" t="s">
-        <v>685</v>
+        <v>751</v>
+      </c>
+      <c r="C86" t="s">
+        <v>652</v>
+      </c>
+      <c r="D86" t="s">
+        <v>746</v>
       </c>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B87" s="5" t="s">
-        <v>688</v>
+        <v>678</v>
       </c>
       <c r="C87" t="s">
         <v>666</v>
@@ -24809,56 +24836,56 @@
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B88" t="s">
-        <v>689</v>
+        <v>680</v>
       </c>
       <c r="C88" t="s">
         <v>652</v>
       </c>
       <c r="D88" t="s">
-        <v>709</v>
+        <v>521</v>
       </c>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B89" t="s">
-        <v>708</v>
-      </c>
-      <c r="C89" t="s">
-        <v>513</v>
+        <v>681</v>
       </c>
       <c r="D89" t="s">
-        <v>710</v>
+        <v>534</v>
       </c>
       <c r="E89" t="s">
-        <v>711</v>
+        <v>684</v>
       </c>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B90" t="s">
-        <v>707</v>
+        <v>686</v>
       </c>
       <c r="E90" t="s">
-        <v>712</v>
+        <v>559</v>
       </c>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B91" t="s">
-        <v>715</v>
+        <v>687</v>
       </c>
       <c r="E91" t="s">
-        <v>713</v>
+        <v>685</v>
       </c>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B92" t="s">
-        <v>716</v>
-      </c>
-      <c r="E92" t="s">
-        <v>714</v>
+        <v>749</v>
+      </c>
+      <c r="C92" t="s">
+        <v>652</v>
+      </c>
+      <c r="D92" t="s">
+        <v>746</v>
       </c>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B93" s="5" t="s">
-        <v>717</v>
+        <v>688</v>
       </c>
       <c r="C93" t="s">
         <v>666</v>
@@ -24872,50 +24899,124 @@
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B94" t="s">
-        <v>718</v>
+        <v>689</v>
       </c>
       <c r="C94" t="s">
         <v>652</v>
       </c>
       <c r="D94" t="s">
-        <v>535</v>
+        <v>709</v>
       </c>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B95" t="s">
-        <v>719</v>
+        <v>708</v>
       </c>
       <c r="C95" t="s">
-        <v>721</v>
+        <v>513</v>
       </c>
       <c r="D95" t="s">
-        <v>691</v>
+        <v>710</v>
+      </c>
+      <c r="E95" t="s">
+        <v>711</v>
       </c>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B96" t="s">
+        <v>707</v>
+      </c>
+      <c r="E96" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B97" t="s">
+        <v>715</v>
+      </c>
+      <c r="E97" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B98" t="s">
+        <v>716</v>
+      </c>
+      <c r="E98" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B99" t="s">
+        <v>748</v>
+      </c>
+      <c r="C99" t="s">
+        <v>652</v>
+      </c>
+      <c r="D99" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="100" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B100" s="5" t="s">
+        <v>717</v>
+      </c>
+      <c r="C100" t="s">
+        <v>666</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>682</v>
+      </c>
+      <c r="E100" s="5" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="101" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B101" t="s">
+        <v>718</v>
+      </c>
+      <c r="C101" t="s">
+        <v>652</v>
+      </c>
+      <c r="D101" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="102" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B102" t="s">
+        <v>719</v>
+      </c>
+      <c r="C102" t="s">
+        <v>721</v>
+      </c>
+      <c r="D102" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="103" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B103" t="s">
         <v>720</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C103" t="s">
         <v>722</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D103" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B99" s="5" t="s">
+    <row r="106" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B106" s="5" t="s">
         <v>532</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C106" t="s">
         <v>690</v>
       </c>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B100" t="s">
+    <row r="107" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B107" t="s">
         <v>698</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C107" t="s">
         <v>699</v>
       </c>
     </row>
@@ -24928,8 +25029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -25009,51 +25110,51 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
+      <c r="A13" s="24" t="s">
         <v>448</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="24" t="s">
         <v>490</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B14" t="s">
+      <c r="B14" s="24" t="s">
         <v>730</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B15" t="s">
+      <c r="B15" s="24" t="s">
         <v>731</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B16" t="s">
+      <c r="B16" s="24" t="s">
         <v>732</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
+      <c r="A17" s="24" t="s">
         <v>449</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="24" t="s">
         <v>733</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B18" t="s">
+      <c r="B18" s="24" t="s">
         <v>734</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B19" t="s">
+      <c r="B19" s="24" t="s">
         <v>735</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A20" t="s">
+      <c r="A20" s="24" t="s">
         <v>736</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="24" t="s">
         <v>737</v>
       </c>
     </row>

</xml_diff>

<commit_message>
0.0.b2.2.2 GUI Class Timezone Selector Commented
</commit_message>
<xml_diff>
--- a/Roadmap.xlsx
+++ b/Roadmap.xlsx
@@ -23924,7 +23924,7 @@
   <dimension ref="A1:L107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -23992,7 +23992,7 @@
       <c r="B4" t="s">
         <v>701</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="24" t="s">
         <v>523</v>
       </c>
       <c r="I4" t="s">
@@ -25022,6 +25022,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
0.0.b2.2.3 GUI Class Radar Selector Commented
</commit_message>
<xml_diff>
--- a/Roadmap.xlsx
+++ b/Roadmap.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="753">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="755">
   <si>
     <t>56 pixels</t>
   </si>
@@ -2295,6 +2295,12 @@
   </si>
   <si>
     <t>0.2.a7</t>
+  </si>
+  <si>
+    <t>0.2.a5</t>
+  </si>
+  <si>
+    <t>Create a master Radar Set that is built off identifying radars, radar select module gets files from that.</t>
   </si>
 </sst>
 </file>
@@ -23921,10 +23927,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L107"/>
+  <dimension ref="A1:L108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -24540,483 +24546,491 @@
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B60" t="s">
-        <v>646</v>
-      </c>
-      <c r="C60" t="s">
-        <v>513</v>
+        <v>753</v>
       </c>
       <c r="D60" t="s">
-        <v>637</v>
-      </c>
-      <c r="E60" t="s">
-        <v>641</v>
+        <v>754</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B61" t="s">
-        <v>647</v>
+        <v>646</v>
+      </c>
+      <c r="C61" t="s">
+        <v>513</v>
+      </c>
+      <c r="D61" t="s">
+        <v>637</v>
       </c>
       <c r="E61" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B62" t="s">
-        <v>648</v>
-      </c>
-      <c r="D62" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="E62" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B63" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D63" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="E63" t="s">
-        <v>111</v>
+        <v>643</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B64" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D64" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="E64" t="s">
-        <v>644</v>
+        <v>111</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B65" t="s">
-        <v>651</v>
+        <v>650</v>
+      </c>
+      <c r="D65" t="s">
+        <v>640</v>
       </c>
       <c r="E65" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B66" t="s">
+        <v>651</v>
+      </c>
+      <c r="E66" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B67" t="s">
         <v>752</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C67" t="s">
         <v>652</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D67" t="s">
         <v>746</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B67" s="5" t="s">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B68" s="5" t="s">
         <v>668</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C68" t="s">
         <v>666</v>
       </c>
-      <c r="D67" s="5" t="s">
+      <c r="D68" s="5" t="s">
         <v>682</v>
       </c>
-      <c r="E67" s="5" t="s">
+      <c r="E68" s="5" t="s">
         <v>683</v>
-      </c>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B68" t="s">
-        <v>530</v>
-      </c>
-      <c r="C68" t="s">
-        <v>652</v>
-      </c>
-      <c r="D68" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B69" t="s">
-        <v>570</v>
+        <v>530</v>
+      </c>
+      <c r="C69" t="s">
+        <v>652</v>
       </c>
       <c r="D69" t="s">
-        <v>517</v>
+        <v>548</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B70" t="s">
-        <v>653</v>
+        <v>570</v>
       </c>
       <c r="D70" t="s">
-        <v>657</v>
+        <v>517</v>
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B71" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D71" t="s">
-        <v>567</v>
+        <v>657</v>
       </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B72" t="s">
-        <v>740</v>
+        <v>654</v>
       </c>
       <c r="D72" t="s">
-        <v>741</v>
+        <v>567</v>
       </c>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B73" t="s">
-        <v>549</v>
-      </c>
-      <c r="C73" t="s">
-        <v>513</v>
+        <v>740</v>
       </c>
       <c r="D73" t="s">
-        <v>655</v>
-      </c>
-      <c r="E73" t="s">
-        <v>659</v>
+        <v>741</v>
       </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B74" t="s">
-        <v>550</v>
+        <v>549</v>
+      </c>
+      <c r="C74" t="s">
+        <v>513</v>
+      </c>
+      <c r="D74" t="s">
+        <v>655</v>
       </c>
       <c r="E74" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B75" t="s">
-        <v>661</v>
-      </c>
-      <c r="D75" t="s">
-        <v>656</v>
+        <v>550</v>
       </c>
       <c r="E75" t="s">
-        <v>669</v>
+        <v>660</v>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B76" t="s">
-        <v>662</v>
+        <v>661</v>
+      </c>
+      <c r="D76" t="s">
+        <v>656</v>
       </c>
       <c r="E76" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B77" t="s">
-        <v>663</v>
-      </c>
-      <c r="D77" t="s">
-        <v>671</v>
+        <v>662</v>
       </c>
       <c r="E77" t="s">
-        <v>111</v>
+        <v>670</v>
       </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B78" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D78" t="s">
-        <v>658</v>
+        <v>671</v>
       </c>
       <c r="E78" t="s">
-        <v>672</v>
+        <v>111</v>
       </c>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B79" t="s">
-        <v>674</v>
+        <v>664</v>
+      </c>
+      <c r="D79" t="s">
+        <v>658</v>
       </c>
       <c r="E79" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B80" t="s">
-        <v>742</v>
-      </c>
-      <c r="D80" t="s">
-        <v>743</v>
+        <v>674</v>
       </c>
       <c r="E80" t="s">
-        <v>744</v>
+        <v>673</v>
       </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B81" t="s">
+        <v>742</v>
+      </c>
+      <c r="D81" t="s">
+        <v>743</v>
+      </c>
+      <c r="E81" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B82" t="s">
         <v>750</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C82" t="s">
         <v>652</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D82" t="s">
         <v>746</v>
       </c>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B82" s="5" t="s">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B83" s="5" t="s">
         <v>675</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C83" t="s">
         <v>666</v>
       </c>
-      <c r="D82" s="5" t="s">
+      <c r="D83" s="5" t="s">
         <v>682</v>
       </c>
-      <c r="E82" s="5" t="s">
+      <c r="E83" s="5" t="s">
         <v>683</v>
-      </c>
-    </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B83" t="s">
-        <v>531</v>
-      </c>
-      <c r="C83" t="s">
-        <v>652</v>
-      </c>
-      <c r="D83" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B84" t="s">
-        <v>676</v>
+        <v>531</v>
+      </c>
+      <c r="C84" t="s">
+        <v>652</v>
       </c>
       <c r="D84" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B85" t="s">
-        <v>533</v>
-      </c>
-      <c r="C85" t="s">
-        <v>513</v>
+        <v>676</v>
       </c>
       <c r="D85" t="s">
-        <v>677</v>
-      </c>
-      <c r="E85" t="s">
-        <v>679</v>
+        <v>520</v>
       </c>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B86" t="s">
+        <v>533</v>
+      </c>
+      <c r="C86" t="s">
+        <v>513</v>
+      </c>
+      <c r="D86" t="s">
+        <v>677</v>
+      </c>
+      <c r="E86" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B87" t="s">
         <v>751</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C87" t="s">
         <v>652</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D87" t="s">
         <v>746</v>
       </c>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B87" s="5" t="s">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B88" s="5" t="s">
         <v>678</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C88" t="s">
         <v>666</v>
       </c>
-      <c r="D87" s="5" t="s">
+      <c r="D88" s="5" t="s">
         <v>682</v>
       </c>
-      <c r="E87" s="5" t="s">
+      <c r="E88" s="5" t="s">
         <v>683</v>
-      </c>
-    </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B88" t="s">
-        <v>680</v>
-      </c>
-      <c r="C88" t="s">
-        <v>652</v>
-      </c>
-      <c r="D88" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B89" t="s">
-        <v>681</v>
+        <v>680</v>
+      </c>
+      <c r="C89" t="s">
+        <v>652</v>
       </c>
       <c r="D89" t="s">
-        <v>534</v>
-      </c>
-      <c r="E89" t="s">
-        <v>684</v>
+        <v>521</v>
       </c>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B90" t="s">
-        <v>686</v>
+        <v>681</v>
+      </c>
+      <c r="D90" t="s">
+        <v>534</v>
       </c>
       <c r="E90" t="s">
-        <v>559</v>
+        <v>684</v>
       </c>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B91" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="E91" t="s">
-        <v>685</v>
+        <v>559</v>
       </c>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B92" t="s">
+        <v>687</v>
+      </c>
+      <c r="E92" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B93" t="s">
         <v>749</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C93" t="s">
         <v>652</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D93" t="s">
         <v>746</v>
       </c>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B93" s="5" t="s">
+    <row r="94" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B94" s="5" t="s">
         <v>688</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C94" t="s">
         <v>666</v>
       </c>
-      <c r="D93" s="5" t="s">
+      <c r="D94" s="5" t="s">
         <v>682</v>
       </c>
-      <c r="E93" s="5" t="s">
+      <c r="E94" s="5" t="s">
         <v>683</v>
-      </c>
-    </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B94" t="s">
-        <v>689</v>
-      </c>
-      <c r="C94" t="s">
-        <v>652</v>
-      </c>
-      <c r="D94" t="s">
-        <v>709</v>
       </c>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B95" t="s">
-        <v>708</v>
+        <v>689</v>
       </c>
       <c r="C95" t="s">
-        <v>513</v>
+        <v>652</v>
       </c>
       <c r="D95" t="s">
-        <v>710</v>
-      </c>
-      <c r="E95" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B96" t="s">
-        <v>707</v>
+        <v>708</v>
+      </c>
+      <c r="C96" t="s">
+        <v>513</v>
+      </c>
+      <c r="D96" t="s">
+        <v>710</v>
       </c>
       <c r="E96" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B97" t="s">
-        <v>715</v>
+        <v>707</v>
       </c>
       <c r="E97" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B98" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="E98" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B99" t="s">
+        <v>716</v>
+      </c>
+      <c r="E99" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="100" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B100" t="s">
         <v>748</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C100" t="s">
         <v>652</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D100" t="s">
         <v>746</v>
       </c>
     </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B100" s="5" t="s">
+    <row r="101" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B101" s="5" t="s">
         <v>717</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C101" t="s">
         <v>666</v>
       </c>
-      <c r="D100" s="5" t="s">
+      <c r="D101" s="5" t="s">
         <v>682</v>
       </c>
-      <c r="E100" s="5" t="s">
+      <c r="E101" s="5" t="s">
         <v>683</v>
-      </c>
-    </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B101" t="s">
-        <v>718</v>
-      </c>
-      <c r="C101" t="s">
-        <v>652</v>
-      </c>
-      <c r="D101" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B102" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C102" t="s">
-        <v>721</v>
+        <v>652</v>
       </c>
       <c r="D102" t="s">
-        <v>691</v>
+        <v>535</v>
       </c>
     </row>
     <row r="103" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B103" t="s">
+        <v>719</v>
+      </c>
+      <c r="C103" t="s">
+        <v>721</v>
+      </c>
+      <c r="D103" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="104" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B104" t="s">
         <v>720</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C104" t="s">
         <v>722</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D104" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="106" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B106" s="5" t="s">
+    <row r="107" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B107" s="5" t="s">
         <v>532</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C107" t="s">
         <v>690</v>
       </c>
     </row>
-    <row r="107" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B107" t="s">
+    <row r="108" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B108" t="s">
         <v>698</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C108" t="s">
         <v>699</v>
       </c>
     </row>

</xml_diff>

<commit_message>
0.0.b2.2.5 GUI Class Main Window Commented
Gui File Finished
</commit_message>
<xml_diff>
--- a/Roadmap.xlsx
+++ b/Roadmap.xlsx
@@ -1730,9 +1730,6 @@
     <t>Track coordinates are out of order</t>
   </si>
   <si>
-    <t>File too short / not enough points</t>
-  </si>
-  <si>
     <t>Sliders are out of whack (end time before start time)</t>
   </si>
   <si>
@@ -2301,6 +2298,9 @@
   </si>
   <si>
     <t>Create a master Radar Set that is built off identifying radars, radar select module gets files from that.</t>
+  </si>
+  <si>
+    <t>File too short / not enough points, either when initially loaded or after trim</t>
   </si>
 </sst>
 </file>
@@ -23929,8 +23929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -23985,7 +23985,7 @@
         <v>513</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I3" t="s">
         <v>497</v>
@@ -23996,7 +23996,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="D4" s="24" t="s">
         <v>523</v>
@@ -24010,10 +24010,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D5" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.4">
@@ -24052,7 +24052,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D8" t="s">
         <v>538</v>
@@ -24069,7 +24069,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D9" t="s">
         <v>539</v>
@@ -24077,7 +24077,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D10" t="s">
         <v>541</v>
@@ -24088,7 +24088,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D11" t="s">
         <v>536</v>
@@ -24099,7 +24099,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E12" t="s">
         <v>556</v>
@@ -24107,7 +24107,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E13" t="s">
         <v>557</v>
@@ -24115,7 +24115,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D14" t="s">
         <v>537</v>
@@ -24126,7 +24126,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E15" t="s">
         <v>559</v>
@@ -24134,7 +24134,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E16" t="s">
         <v>560</v>
@@ -24142,15 +24142,15 @@
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B17" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E17" t="s">
-        <v>564</v>
+        <v>754</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B18" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E18" t="s">
         <v>561</v>
@@ -24158,7 +24158,7 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B19" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="E19" t="s">
         <v>562</v>
@@ -24166,7 +24166,7 @@
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B20" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="E20" t="s">
         <v>563</v>
@@ -24174,257 +24174,257 @@
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D21" t="s">
         <v>540</v>
       </c>
       <c r="E21" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B22" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E22" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="E23" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D24" t="s">
         <v>543</v>
       </c>
       <c r="E24" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E25" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B26" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E26" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D27" t="s">
         <v>544</v>
       </c>
       <c r="E27" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E28" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E29" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D30" t="s">
         <v>545</v>
       </c>
       <c r="E30" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B31" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="E31" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E32" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E33" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B34" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E34" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B35" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="E35" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B36" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D36" t="s">
         <v>546</v>
       </c>
       <c r="E36" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B37" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D37" t="s">
         <v>547</v>
       </c>
       <c r="E37" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="E38" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B39" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="E39" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B40" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="E40" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B41" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="E41" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B42" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E42" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B43" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D43" t="s">
         <v>551</v>
       </c>
       <c r="E43" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B44" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="C44" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D44" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B45" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C45" t="s">
         <v>513</v>
       </c>
       <c r="D45" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E45" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B46" t="s">
+        <v>744</v>
+      </c>
+      <c r="C46" t="s">
+        <v>651</v>
+      </c>
+      <c r="D46" t="s">
         <v>745</v>
-      </c>
-      <c r="C46" t="s">
-        <v>652</v>
-      </c>
-      <c r="D46" t="s">
-        <v>746</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B47" s="5" t="s">
+        <v>664</v>
+      </c>
+      <c r="C47" t="s">
         <v>665</v>
       </c>
-      <c r="C47" t="s">
-        <v>666</v>
-      </c>
       <c r="D47" s="5" t="s">
+        <v>681</v>
+      </c>
+      <c r="E47" s="5" t="s">
         <v>682</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.4">
@@ -24432,7 +24432,7 @@
         <v>514</v>
       </c>
       <c r="C48" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D48" t="s">
         <v>515</v>
@@ -24440,73 +24440,73 @@
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B49" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C49" t="s">
         <v>513</v>
       </c>
       <c r="D49" t="s">
+        <v>625</v>
+      </c>
+      <c r="E49" t="s">
         <v>626</v>
-      </c>
-      <c r="E49" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B50" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="E50" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B51" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E51" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B52" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="E52" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B53" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="E53" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B54" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C54" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D54" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B55" s="5" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C55" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="D55" s="5" t="s">
+        <v>681</v>
+      </c>
+      <c r="E55" s="5" t="s">
         <v>682</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.4">
@@ -24514,7 +24514,7 @@
         <v>526</v>
       </c>
       <c r="C56" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D56" t="s">
         <v>516</v>
@@ -24530,7 +24530,7 @@
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B58" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D58" t="s">
         <v>522</v>
@@ -24538,7 +24538,7 @@
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B59" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D59" t="s">
         <v>542</v>
@@ -24546,51 +24546,51 @@
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B60" t="s">
+        <v>752</v>
+      </c>
+      <c r="D60" t="s">
         <v>753</v>
-      </c>
-      <c r="D60" t="s">
-        <v>754</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B61" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C61" t="s">
         <v>513</v>
       </c>
       <c r="D61" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="E61" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B62" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="E62" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B63" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D63" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="E63" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B64" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D64" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="E64" t="s">
         <v>111</v>
@@ -24598,46 +24598,46 @@
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B65" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D65" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="E65" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B66" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="E66" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B67" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="C67" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D67" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B68" s="5" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C68" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="D68" s="5" t="s">
+        <v>681</v>
+      </c>
+      <c r="E68" s="5" t="s">
         <v>682</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.4">
@@ -24645,7 +24645,7 @@
         <v>530</v>
       </c>
       <c r="C69" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D69" t="s">
         <v>548</v>
@@ -24653,7 +24653,7 @@
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B70" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D70" t="s">
         <v>517</v>
@@ -24661,26 +24661,26 @@
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B71" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="D71" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B72" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D72" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B73" t="s">
+        <v>739</v>
+      </c>
+      <c r="D73" t="s">
         <v>740</v>
-      </c>
-      <c r="D73" t="s">
-        <v>741</v>
       </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.4">
@@ -24691,10 +24691,10 @@
         <v>513</v>
       </c>
       <c r="D74" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="E74" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.4">
@@ -24702,34 +24702,34 @@
         <v>550</v>
       </c>
       <c r="E75" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B76" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D76" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="E76" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B77" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="E77" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B78" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D78" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="E78" t="s">
         <v>111</v>
@@ -24737,57 +24737,57 @@
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B79" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D79" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E79" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B80" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="E80" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B81" t="s">
+        <v>741</v>
+      </c>
+      <c r="D81" t="s">
         <v>742</v>
       </c>
-      <c r="D81" t="s">
+      <c r="E81" t="s">
         <v>743</v>
-      </c>
-      <c r="E81" t="s">
-        <v>744</v>
       </c>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B82" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C82" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D82" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B83" s="5" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="C83" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="D83" s="5" t="s">
+        <v>681</v>
+      </c>
+      <c r="E83" s="5" t="s">
         <v>682</v>
-      </c>
-      <c r="E83" s="5" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.4">
@@ -24795,7 +24795,7 @@
         <v>531</v>
       </c>
       <c r="C84" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D84" t="s">
         <v>519</v>
@@ -24803,7 +24803,7 @@
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B85" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="D85" t="s">
         <v>520</v>
@@ -24817,43 +24817,43 @@
         <v>513</v>
       </c>
       <c r="D86" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="E86" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B87" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="C87" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D87" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B88" s="5" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="C88" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="D88" s="5" t="s">
+        <v>681</v>
+      </c>
+      <c r="E88" s="5" t="s">
         <v>682</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B89" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="C89" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D89" t="s">
         <v>521</v>
@@ -24861,18 +24861,18 @@
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B90" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="D90" t="s">
         <v>534</v>
       </c>
       <c r="E90" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B91" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="E91" t="s">
         <v>559</v>
@@ -24880,117 +24880,117 @@
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B92" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="E92" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B93" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="C93" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D93" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B94" s="5" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C94" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="D94" s="5" t="s">
+        <v>681</v>
+      </c>
+      <c r="E94" s="5" t="s">
         <v>682</v>
-      </c>
-      <c r="E94" s="5" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B95" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C95" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D95" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B96" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="C96" t="s">
         <v>513</v>
       </c>
       <c r="D96" t="s">
+        <v>709</v>
+      </c>
+      <c r="E96" t="s">
         <v>710</v>
-      </c>
-      <c r="E96" t="s">
-        <v>711</v>
       </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B97" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E97" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B98" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="E98" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B99" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="E99" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B100" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C100" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D100" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="101" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B101" s="5" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="C101" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="D101" s="5" t="s">
+        <v>681</v>
+      </c>
+      <c r="E101" s="5" t="s">
         <v>682</v>
-      </c>
-      <c r="E101" s="5" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B102" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C102" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D102" t="s">
         <v>535</v>
@@ -24998,24 +24998,24 @@
     </row>
     <row r="103" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B103" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C103" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="D103" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B104" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C104" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="D104" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="107" spans="2:5" x14ac:dyDescent="0.4">
@@ -25023,15 +25023,15 @@
         <v>532</v>
       </c>
       <c r="C107" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="108" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B108" t="s">
+        <v>697</v>
+      </c>
+      <c r="C108" t="s">
         <v>698</v>
-      </c>
-      <c r="C108" t="s">
-        <v>699</v>
       </c>
     </row>
   </sheetData>
@@ -25055,24 +25055,24 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>703</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="24" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B2" s="24"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="24" t="s">
+        <v>725</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>726</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>727</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
@@ -25083,33 +25083,33 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" s="24" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B6" s="24" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B7" s="24" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B8" s="24" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" s="24" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.4">
@@ -25121,7 +25121,7 @@
     <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" s="24"/>
       <c r="B11" s="24" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.4">
@@ -25134,17 +25134,17 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B14" s="24" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B15" s="24" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B16" s="24" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.4">
@@ -25152,25 +25152,25 @@
         <v>449</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B18" s="24" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B19" s="24" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A20" s="24" t="s">
+        <v>735</v>
+      </c>
+      <c r="B20" s="24" t="s">
         <v>736</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>737</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
0.0.b2.2.6 GUI Class Main Window Commented
All module commented
</commit_message>
<xml_diff>
--- a/Roadmap.xlsx
+++ b/Roadmap.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="755">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="758">
   <si>
     <t>56 pixels</t>
   </si>
@@ -1655,9 +1655,6 @@
     <t>Reroute stdout to Textbox</t>
   </si>
   <si>
-    <t>Code in general details</t>
-  </si>
-  <si>
     <t>Test Trim Gui</t>
   </si>
   <si>
@@ -2141,9 +2138,6 @@
     <t>0.0.b2.1</t>
   </si>
   <si>
-    <t>Comment all Code</t>
-  </si>
-  <si>
     <t>Headings</t>
   </si>
   <si>
@@ -2301,6 +2295,21 @@
   </si>
   <si>
     <t>File too short / not enough points, either when initially loaded or after trim</t>
+  </si>
+  <si>
+    <t>0.0.b40.1</t>
+  </si>
+  <si>
+    <t>Test Clicking Media and Radar Buttons</t>
+  </si>
+  <si>
+    <t>If buttons are clicked out of order</t>
+  </si>
+  <si>
+    <t>Comment all Code (currently up to KML Creator)</t>
+  </si>
+  <si>
+    <t>Code in general details (frame in GUI)</t>
   </si>
 </sst>
 </file>
@@ -23927,10 +23936,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L108"/>
+  <dimension ref="A1:L109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -23951,10 +23960,10 @@
         <v>493</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>552</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>553</v>
       </c>
       <c r="I1" t="s">
         <v>494</v>
@@ -23985,7 +23994,7 @@
         <v>513</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I3" t="s">
         <v>497</v>
@@ -23996,7 +24005,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D4" s="24" t="s">
         <v>523</v>
@@ -24010,10 +24019,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="D5" t="s">
-        <v>701</v>
+        <v>756</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.4">
@@ -24052,7 +24061,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D8" t="s">
         <v>538</v>
@@ -24069,323 +24078,323 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D9" t="s">
-        <v>539</v>
+        <v>757</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D10" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="E10" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D11" t="s">
         <v>536</v>
       </c>
       <c r="E11" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E12" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E13" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D14" t="s">
         <v>537</v>
       </c>
       <c r="E14" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E15" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E16" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B17" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E17" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B18" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E18" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B19" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E19" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B20" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="E20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D21" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="E21" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B22" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="E22" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E23" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="D24" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E24" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="E25" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B26" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E26" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D27" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="E27" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E28" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E29" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D30" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E30" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B31" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="E31" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="E32" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E33" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B34" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E34" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B35" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E35" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B36" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D36" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E36" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B37" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D37" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E37" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="E38" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B39" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="E39" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B40" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="E40" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B41" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="E41" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B42" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="E42" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B43" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D43" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E43" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B44" t="s">
-        <v>693</v>
-      </c>
-      <c r="C44" t="s">
-        <v>651</v>
+        <v>753</v>
       </c>
       <c r="D44" t="s">
-        <v>691</v>
+        <v>754</v>
+      </c>
+      <c r="E44" t="s">
+        <v>755</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.4">
@@ -24393,645 +24402,656 @@
         <v>692</v>
       </c>
       <c r="C45" t="s">
-        <v>513</v>
+        <v>650</v>
       </c>
       <c r="D45" t="s">
-        <v>695</v>
-      </c>
-      <c r="E45" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B46" t="s">
-        <v>744</v>
+        <v>691</v>
       </c>
       <c r="C46" t="s">
-        <v>651</v>
+        <v>513</v>
       </c>
       <c r="D46" t="s">
-        <v>745</v>
+        <v>694</v>
+      </c>
+      <c r="E46" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B47" s="5" t="s">
+      <c r="B47" t="s">
+        <v>742</v>
+      </c>
+      <c r="C47" t="s">
+        <v>650</v>
+      </c>
+      <c r="D47" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B48" s="5" t="s">
+        <v>663</v>
+      </c>
+      <c r="C48" t="s">
         <v>664</v>
       </c>
-      <c r="C47" t="s">
-        <v>665</v>
-      </c>
-      <c r="D47" s="5" t="s">
+      <c r="D48" s="5" t="s">
+        <v>680</v>
+      </c>
+      <c r="E48" s="5" t="s">
         <v>681</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B48" t="s">
-        <v>514</v>
-      </c>
-      <c r="C48" t="s">
-        <v>651</v>
-      </c>
-      <c r="D48" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B49" t="s">
-        <v>631</v>
+        <v>514</v>
       </c>
       <c r="C49" t="s">
-        <v>513</v>
+        <v>650</v>
       </c>
       <c r="D49" t="s">
-        <v>625</v>
-      </c>
-      <c r="E49" t="s">
-        <v>626</v>
+        <v>515</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B50" t="s">
-        <v>632</v>
+        <v>630</v>
+      </c>
+      <c r="C50" t="s">
+        <v>513</v>
+      </c>
+      <c r="D50" t="s">
+        <v>624</v>
       </c>
       <c r="E50" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B51" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="E51" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B52" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="E52" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B53" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="E53" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B54" t="s">
-        <v>746</v>
-      </c>
-      <c r="C54" t="s">
-        <v>651</v>
-      </c>
-      <c r="D54" t="s">
-        <v>745</v>
+        <v>634</v>
+      </c>
+      <c r="E54" t="s">
+        <v>629</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B55" s="5" t="s">
-        <v>666</v>
+      <c r="B55" t="s">
+        <v>744</v>
       </c>
       <c r="C55" t="s">
+        <v>650</v>
+      </c>
+      <c r="D55" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B56" s="5" t="s">
         <v>665</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="C56" t="s">
+        <v>664</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>680</v>
+      </c>
+      <c r="E56" s="5" t="s">
         <v>681</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B56" t="s">
-        <v>526</v>
-      </c>
-      <c r="C56" t="s">
-        <v>651</v>
-      </c>
-      <c r="D56" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B57" t="s">
-        <v>529</v>
+        <v>526</v>
+      </c>
+      <c r="C57" t="s">
+        <v>650</v>
       </c>
       <c r="D57" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B58" t="s">
-        <v>567</v>
+        <v>529</v>
       </c>
       <c r="D58" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B59" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="D59" t="s">
-        <v>542</v>
+        <v>522</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B60" t="s">
-        <v>752</v>
+        <v>567</v>
       </c>
       <c r="D60" t="s">
-        <v>753</v>
+        <v>541</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B61" t="s">
-        <v>645</v>
-      </c>
-      <c r="C61" t="s">
-        <v>513</v>
+        <v>750</v>
       </c>
       <c r="D61" t="s">
-        <v>636</v>
-      </c>
-      <c r="E61" t="s">
-        <v>640</v>
+        <v>751</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B62" t="s">
-        <v>646</v>
+        <v>644</v>
+      </c>
+      <c r="C62" t="s">
+        <v>513</v>
+      </c>
+      <c r="D62" t="s">
+        <v>635</v>
       </c>
       <c r="E62" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B63" t="s">
-        <v>647</v>
-      </c>
-      <c r="D63" t="s">
-        <v>637</v>
+        <v>645</v>
       </c>
       <c r="E63" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B64" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="D64" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="E64" t="s">
-        <v>111</v>
+        <v>641</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B65" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="D65" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="E65" t="s">
-        <v>643</v>
+        <v>111</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B66" t="s">
-        <v>650</v>
+        <v>648</v>
+      </c>
+      <c r="D66" t="s">
+        <v>638</v>
       </c>
       <c r="E66" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B67" t="s">
-        <v>751</v>
-      </c>
-      <c r="C67" t="s">
-        <v>651</v>
-      </c>
-      <c r="D67" t="s">
-        <v>745</v>
+        <v>649</v>
+      </c>
+      <c r="E67" t="s">
+        <v>643</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B68" s="5" t="s">
-        <v>667</v>
+      <c r="B68" t="s">
+        <v>749</v>
       </c>
       <c r="C68" t="s">
-        <v>665</v>
-      </c>
-      <c r="D68" s="5" t="s">
+        <v>650</v>
+      </c>
+      <c r="D68" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B69" s="5" t="s">
+        <v>666</v>
+      </c>
+      <c r="C69" t="s">
+        <v>664</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>680</v>
+      </c>
+      <c r="E69" s="5" t="s">
         <v>681</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B69" t="s">
-        <v>530</v>
-      </c>
-      <c r="C69" t="s">
-        <v>651</v>
-      </c>
-      <c r="D69" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B70" t="s">
-        <v>569</v>
+        <v>530</v>
+      </c>
+      <c r="C70" t="s">
+        <v>650</v>
       </c>
       <c r="D70" t="s">
-        <v>517</v>
+        <v>547</v>
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B71" t="s">
-        <v>652</v>
+        <v>568</v>
       </c>
       <c r="D71" t="s">
-        <v>656</v>
+        <v>517</v>
       </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B72" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D72" t="s">
-        <v>566</v>
+        <v>655</v>
       </c>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B73" t="s">
-        <v>739</v>
+        <v>652</v>
       </c>
       <c r="D73" t="s">
-        <v>740</v>
+        <v>565</v>
       </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B74" t="s">
-        <v>549</v>
-      </c>
-      <c r="C74" t="s">
-        <v>513</v>
+        <v>737</v>
       </c>
       <c r="D74" t="s">
-        <v>654</v>
-      </c>
-      <c r="E74" t="s">
-        <v>658</v>
+        <v>738</v>
       </c>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B75" t="s">
-        <v>550</v>
+        <v>548</v>
+      </c>
+      <c r="C75" t="s">
+        <v>513</v>
+      </c>
+      <c r="D75" t="s">
+        <v>653</v>
       </c>
       <c r="E75" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B76" t="s">
-        <v>660</v>
-      </c>
-      <c r="D76" t="s">
-        <v>655</v>
+        <v>549</v>
       </c>
       <c r="E76" t="s">
-        <v>668</v>
+        <v>658</v>
       </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B77" t="s">
-        <v>661</v>
+        <v>659</v>
+      </c>
+      <c r="D77" t="s">
+        <v>654</v>
       </c>
       <c r="E77" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B78" t="s">
-        <v>662</v>
-      </c>
-      <c r="D78" t="s">
-        <v>670</v>
+        <v>660</v>
       </c>
       <c r="E78" t="s">
-        <v>111</v>
+        <v>668</v>
       </c>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B79" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="D79" t="s">
-        <v>657</v>
+        <v>669</v>
       </c>
       <c r="E79" t="s">
-        <v>671</v>
+        <v>111</v>
       </c>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B80" t="s">
-        <v>673</v>
+        <v>662</v>
+      </c>
+      <c r="D80" t="s">
+        <v>656</v>
       </c>
       <c r="E80" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B81" t="s">
-        <v>741</v>
-      </c>
-      <c r="D81" t="s">
-        <v>742</v>
+        <v>672</v>
       </c>
       <c r="E81" t="s">
-        <v>743</v>
+        <v>671</v>
       </c>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B82" t="s">
-        <v>749</v>
-      </c>
-      <c r="C82" t="s">
-        <v>651</v>
+        <v>739</v>
       </c>
       <c r="D82" t="s">
-        <v>745</v>
+        <v>740</v>
+      </c>
+      <c r="E82" t="s">
+        <v>741</v>
       </c>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B83" s="5" t="s">
-        <v>674</v>
+      <c r="B83" t="s">
+        <v>747</v>
       </c>
       <c r="C83" t="s">
-        <v>665</v>
-      </c>
-      <c r="D83" s="5" t="s">
+        <v>650</v>
+      </c>
+      <c r="D83" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B84" s="5" t="s">
+        <v>673</v>
+      </c>
+      <c r="C84" t="s">
+        <v>664</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>680</v>
+      </c>
+      <c r="E84" s="5" t="s">
         <v>681</v>
-      </c>
-      <c r="E83" s="5" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B84" t="s">
-        <v>531</v>
-      </c>
-      <c r="C84" t="s">
-        <v>651</v>
-      </c>
-      <c r="D84" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B85" t="s">
-        <v>675</v>
+        <v>531</v>
+      </c>
+      <c r="C85" t="s">
+        <v>650</v>
       </c>
       <c r="D85" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B86" t="s">
-        <v>533</v>
-      </c>
-      <c r="C86" t="s">
-        <v>513</v>
+        <v>674</v>
       </c>
       <c r="D86" t="s">
-        <v>676</v>
-      </c>
-      <c r="E86" t="s">
-        <v>678</v>
+        <v>520</v>
       </c>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B87" t="s">
-        <v>750</v>
+        <v>533</v>
       </c>
       <c r="C87" t="s">
-        <v>651</v>
+        <v>513</v>
       </c>
       <c r="D87" t="s">
-        <v>745</v>
+        <v>675</v>
+      </c>
+      <c r="E87" t="s">
+        <v>677</v>
       </c>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B88" s="5" t="s">
-        <v>677</v>
+      <c r="B88" t="s">
+        <v>748</v>
       </c>
       <c r="C88" t="s">
-        <v>665</v>
-      </c>
-      <c r="D88" s="5" t="s">
+        <v>650</v>
+      </c>
+      <c r="D88" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B89" s="5" t="s">
+        <v>676</v>
+      </c>
+      <c r="C89" t="s">
+        <v>664</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>680</v>
+      </c>
+      <c r="E89" s="5" t="s">
         <v>681</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B89" t="s">
-        <v>679</v>
-      </c>
-      <c r="C89" t="s">
-        <v>651</v>
-      </c>
-      <c r="D89" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B90" t="s">
-        <v>680</v>
+        <v>678</v>
+      </c>
+      <c r="C90" t="s">
+        <v>650</v>
       </c>
       <c r="D90" t="s">
-        <v>534</v>
-      </c>
-      <c r="E90" t="s">
-        <v>683</v>
+        <v>521</v>
       </c>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B91" t="s">
-        <v>685</v>
+        <v>679</v>
+      </c>
+      <c r="D91" t="s">
+        <v>534</v>
       </c>
       <c r="E91" t="s">
-        <v>559</v>
+        <v>682</v>
       </c>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B92" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="E92" t="s">
-        <v>684</v>
+        <v>558</v>
       </c>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B93" t="s">
-        <v>748</v>
-      </c>
-      <c r="C93" t="s">
-        <v>651</v>
-      </c>
-      <c r="D93" t="s">
-        <v>745</v>
+        <v>685</v>
+      </c>
+      <c r="E93" t="s">
+        <v>683</v>
       </c>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B94" s="5" t="s">
-        <v>687</v>
+      <c r="B94" t="s">
+        <v>746</v>
       </c>
       <c r="C94" t="s">
-        <v>665</v>
-      </c>
-      <c r="D94" s="5" t="s">
+        <v>650</v>
+      </c>
+      <c r="D94" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B95" s="5" t="s">
+        <v>686</v>
+      </c>
+      <c r="C95" t="s">
+        <v>664</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>680</v>
+      </c>
+      <c r="E95" s="5" t="s">
         <v>681</v>
-      </c>
-      <c r="E94" s="5" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B95" t="s">
-        <v>688</v>
-      </c>
-      <c r="C95" t="s">
-        <v>651</v>
-      </c>
-      <c r="D95" t="s">
-        <v>708</v>
       </c>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B96" t="s">
-        <v>707</v>
+        <v>687</v>
       </c>
       <c r="C96" t="s">
-        <v>513</v>
+        <v>650</v>
       </c>
       <c r="D96" t="s">
-        <v>709</v>
-      </c>
-      <c r="E96" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B97" t="s">
-        <v>706</v>
+        <v>705</v>
+      </c>
+      <c r="C97" t="s">
+        <v>513</v>
+      </c>
+      <c r="D97" t="s">
+        <v>707</v>
       </c>
       <c r="E97" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B98" t="s">
-        <v>714</v>
+        <v>704</v>
       </c>
       <c r="E98" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B99" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="E99" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B100" t="s">
-        <v>747</v>
-      </c>
-      <c r="C100" t="s">
-        <v>651</v>
-      </c>
-      <c r="D100" t="s">
+        <v>713</v>
+      </c>
+      <c r="E100" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="101" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B101" t="s">
         <v>745</v>
       </c>
-    </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B101" s="5" t="s">
-        <v>716</v>
-      </c>
       <c r="C101" t="s">
-        <v>665</v>
-      </c>
-      <c r="D101" s="5" t="s">
+        <v>650</v>
+      </c>
+      <c r="D101" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="102" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B102" s="5" t="s">
+        <v>714</v>
+      </c>
+      <c r="C102" t="s">
+        <v>664</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>680</v>
+      </c>
+      <c r="E102" s="5" t="s">
         <v>681</v>
-      </c>
-      <c r="E101" s="5" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B102" t="s">
-        <v>717</v>
-      </c>
-      <c r="C102" t="s">
-        <v>651</v>
-      </c>
-      <c r="D102" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="103" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B103" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="C103" t="s">
-        <v>720</v>
+        <v>650</v>
       </c>
       <c r="D103" t="s">
-        <v>690</v>
+        <v>535</v>
       </c>
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B104" t="s">
+        <v>716</v>
+      </c>
+      <c r="C104" t="s">
+        <v>718</v>
+      </c>
+      <c r="D104" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="105" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B105" t="s">
+        <v>717</v>
+      </c>
+      <c r="C105" t="s">
         <v>719</v>
       </c>
-      <c r="C104" t="s">
-        <v>721</v>
-      </c>
-      <c r="D104" t="s">
+      <c r="D105" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B108" s="5" t="s">
+        <v>532</v>
+      </c>
+      <c r="C108" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B109" t="s">
         <v>696</v>
       </c>
-    </row>
-    <row r="107" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B107" s="5" t="s">
-        <v>532</v>
-      </c>
-      <c r="C107" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="108" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B108" t="s">
+      <c r="C109" t="s">
         <v>697</v>
-      </c>
-      <c r="C108" t="s">
-        <v>698</v>
       </c>
     </row>
   </sheetData>
@@ -25055,24 +25075,24 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="24" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="B2" s="24"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="24" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
@@ -25083,33 +25103,33 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" s="24" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B6" s="24" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B7" s="24" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B8" s="24" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" s="24" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.4">
@@ -25121,7 +25141,7 @@
     <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" s="24"/>
       <c r="B11" s="24" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.4">
@@ -25134,17 +25154,17 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B14" s="24" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B15" s="24" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B16" s="24" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.4">
@@ -25152,25 +25172,25 @@
         <v>449</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B18" s="24" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B19" s="24" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A20" s="24" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
0.0.b3 Implement default time zone selection and user feedback for selection change
Default Time Zone is selected to be Melbourne. Also implemented feedback through tb when user changes time zone.
</commit_message>
<xml_diff>
--- a/Roadmap.xlsx
+++ b/Roadmap.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="758">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="760">
   <si>
     <t>56 pixels</t>
   </si>
@@ -1610,9 +1610,6 @@
     <t>Clean Up Code</t>
   </si>
   <si>
-    <t>Default TZ selection to Melbourne</t>
-  </si>
-  <si>
     <t>Troubleshoot time code for videos (no seconds)</t>
   </si>
   <si>
@@ -2310,6 +2307,15 @@
   </si>
   <si>
     <t>Code in general details (frame in GUI)</t>
+  </si>
+  <si>
+    <t>0.0.b44</t>
+  </si>
+  <si>
+    <t>Default TZ selection to Melbourne (already done)</t>
+  </si>
+  <si>
+    <t>Fix multiple "Other" options in Timezone Region, also press ok without selecting location, only region</t>
   </si>
 </sst>
 </file>
@@ -2509,7 +2515,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2539,6 +2545,7 @@
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -23936,10 +23943,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L109"/>
+  <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -23960,10 +23967,10 @@
         <v>493</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>551</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>552</v>
       </c>
       <c r="I1" t="s">
         <v>494</v>
@@ -23994,7 +24001,7 @@
         <v>513</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I3" t="s">
         <v>497</v>
@@ -24005,7 +24012,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="D4" s="24" t="s">
         <v>523</v>
@@ -24019,18 +24026,18 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>698</v>
-      </c>
-      <c r="D5" t="s">
-        <v>756</v>
+        <v>697</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>755</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D6" t="s">
-        <v>524</v>
+        <v>758</v>
       </c>
       <c r="I6" t="s">
         <v>505</v>
@@ -24044,10 +24051,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D7" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="I7" t="s">
         <v>506</v>
@@ -24061,10 +24068,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="I8" t="s">
         <v>504</v>
@@ -24078,980 +24085,991 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D9" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D10" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="E10" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D11" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E11" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E12" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E13" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D14" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E14" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E15" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E16" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B17" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E17" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B18" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E18" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B19" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E19" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B20" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E20" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D21" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E21" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B22" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="E22" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="E23" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D24" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="E24" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="E25" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B26" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="E26" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D27" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E27" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E28" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E29" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D30" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="E30" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B31" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E31" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="E32" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="E33" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B34" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E34" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B35" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E35" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B36" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D36" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E36" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B37" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D37" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E37" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E38" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B39" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="E39" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B40" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="E40" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B41" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="E41" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B42" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="E42" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B43" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D43" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="E43" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B44" t="s">
+        <v>752</v>
+      </c>
+      <c r="D44" t="s">
         <v>753</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>754</v>
-      </c>
-      <c r="E44" t="s">
-        <v>755</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B45" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C45" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D45" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B46" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C46" t="s">
         <v>513</v>
       </c>
       <c r="D46" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="E46" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B47" t="s">
+        <v>741</v>
+      </c>
+      <c r="C47" t="s">
+        <v>649</v>
+      </c>
+      <c r="D47" t="s">
         <v>742</v>
       </c>
-      <c r="C47" t="s">
-        <v>650</v>
-      </c>
-      <c r="D47" t="s">
-        <v>743</v>
-      </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B48" s="5" t="s">
+      <c r="B48" t="s">
+        <v>757</v>
+      </c>
+      <c r="C48" t="s">
+        <v>513</v>
+      </c>
+      <c r="D48" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B49" s="5" t="s">
+        <v>662</v>
+      </c>
+      <c r="C49" t="s">
         <v>663</v>
       </c>
-      <c r="C48" t="s">
-        <v>664</v>
-      </c>
-      <c r="D48" s="5" t="s">
+      <c r="D49" s="5" t="s">
+        <v>679</v>
+      </c>
+      <c r="E49" s="5" t="s">
         <v>680</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B49" t="s">
-        <v>514</v>
-      </c>
-      <c r="C49" t="s">
-        <v>650</v>
-      </c>
-      <c r="D49" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B50" t="s">
-        <v>630</v>
+        <v>514</v>
       </c>
       <c r="C50" t="s">
-        <v>513</v>
+        <v>649</v>
       </c>
       <c r="D50" t="s">
-        <v>624</v>
-      </c>
-      <c r="E50" t="s">
-        <v>625</v>
+        <v>515</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B51" t="s">
-        <v>631</v>
+        <v>629</v>
+      </c>
+      <c r="C51" t="s">
+        <v>513</v>
+      </c>
+      <c r="D51" t="s">
+        <v>623</v>
       </c>
       <c r="E51" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B52" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="E52" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B53" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="E53" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B54" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="E54" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B55" t="s">
-        <v>744</v>
-      </c>
-      <c r="C55" t="s">
-        <v>650</v>
-      </c>
-      <c r="D55" t="s">
+        <v>633</v>
+      </c>
+      <c r="E55" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B56" t="s">
         <v>743</v>
       </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B56" s="5" t="s">
-        <v>665</v>
-      </c>
       <c r="C56" t="s">
+        <v>649</v>
+      </c>
+      <c r="D56" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B57" s="5" t="s">
         <v>664</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="C57" t="s">
+        <v>663</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>679</v>
+      </c>
+      <c r="E57" s="5" t="s">
         <v>680</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B57" t="s">
-        <v>526</v>
-      </c>
-      <c r="C57" t="s">
-        <v>650</v>
-      </c>
-      <c r="D57" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B58" t="s">
-        <v>529</v>
+        <v>525</v>
+      </c>
+      <c r="C58" t="s">
+        <v>649</v>
       </c>
       <c r="D58" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B59" t="s">
-        <v>566</v>
+        <v>528</v>
       </c>
       <c r="D59" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B60" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="D60" t="s">
-        <v>541</v>
+        <v>522</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B61" t="s">
-        <v>750</v>
+        <v>566</v>
       </c>
       <c r="D61" t="s">
-        <v>751</v>
+        <v>540</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B62" t="s">
-        <v>644</v>
-      </c>
-      <c r="C62" t="s">
-        <v>513</v>
+        <v>749</v>
       </c>
       <c r="D62" t="s">
-        <v>635</v>
-      </c>
-      <c r="E62" t="s">
-        <v>639</v>
+        <v>750</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B63" t="s">
-        <v>645</v>
+        <v>643</v>
+      </c>
+      <c r="C63" t="s">
+        <v>513</v>
+      </c>
+      <c r="D63" t="s">
+        <v>634</v>
       </c>
       <c r="E63" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B64" t="s">
-        <v>646</v>
-      </c>
-      <c r="D64" t="s">
-        <v>636</v>
+        <v>644</v>
       </c>
       <c r="E64" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B65" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D65" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="E65" t="s">
-        <v>111</v>
+        <v>640</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B66" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="D66" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="E66" t="s">
-        <v>642</v>
+        <v>111</v>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B67" t="s">
-        <v>649</v>
+        <v>647</v>
+      </c>
+      <c r="D67" t="s">
+        <v>637</v>
       </c>
       <c r="E67" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B68" t="s">
-        <v>749</v>
-      </c>
-      <c r="C68" t="s">
-        <v>650</v>
-      </c>
-      <c r="D68" t="s">
-        <v>743</v>
+        <v>648</v>
+      </c>
+      <c r="E68" t="s">
+        <v>642</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B69" s="5" t="s">
-        <v>666</v>
+      <c r="B69" t="s">
+        <v>748</v>
       </c>
       <c r="C69" t="s">
-        <v>664</v>
-      </c>
-      <c r="D69" s="5" t="s">
+        <v>649</v>
+      </c>
+      <c r="D69" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B70" s="5" t="s">
+        <v>665</v>
+      </c>
+      <c r="C70" t="s">
+        <v>663</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>679</v>
+      </c>
+      <c r="E70" s="5" t="s">
         <v>680</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B70" t="s">
-        <v>530</v>
-      </c>
-      <c r="C70" t="s">
-        <v>650</v>
-      </c>
-      <c r="D70" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B71" t="s">
-        <v>568</v>
+        <v>529</v>
+      </c>
+      <c r="C71" t="s">
+        <v>649</v>
       </c>
       <c r="D71" t="s">
-        <v>517</v>
+        <v>546</v>
       </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B72" t="s">
-        <v>651</v>
+        <v>567</v>
       </c>
       <c r="D72" t="s">
-        <v>655</v>
+        <v>517</v>
       </c>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B73" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="D73" t="s">
-        <v>565</v>
+        <v>654</v>
       </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B74" t="s">
-        <v>737</v>
+        <v>651</v>
       </c>
       <c r="D74" t="s">
-        <v>738</v>
+        <v>564</v>
       </c>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B75" t="s">
-        <v>548</v>
-      </c>
-      <c r="C75" t="s">
-        <v>513</v>
+        <v>736</v>
       </c>
       <c r="D75" t="s">
-        <v>653</v>
-      </c>
-      <c r="E75" t="s">
-        <v>657</v>
+        <v>737</v>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B76" t="s">
-        <v>549</v>
+        <v>547</v>
+      </c>
+      <c r="C76" t="s">
+        <v>513</v>
+      </c>
+      <c r="D76" t="s">
+        <v>652</v>
       </c>
       <c r="E76" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B77" t="s">
-        <v>659</v>
-      </c>
-      <c r="D77" t="s">
-        <v>654</v>
+        <v>548</v>
       </c>
       <c r="E77" t="s">
-        <v>667</v>
+        <v>657</v>
       </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B78" t="s">
-        <v>660</v>
+        <v>658</v>
+      </c>
+      <c r="D78" t="s">
+        <v>653</v>
       </c>
       <c r="E78" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B79" t="s">
-        <v>661</v>
-      </c>
-      <c r="D79" t="s">
-        <v>669</v>
+        <v>659</v>
       </c>
       <c r="E79" t="s">
-        <v>111</v>
+        <v>667</v>
       </c>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B80" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="D80" t="s">
-        <v>656</v>
+        <v>668</v>
       </c>
       <c r="E80" t="s">
-        <v>670</v>
+        <v>111</v>
       </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B81" t="s">
-        <v>672</v>
+        <v>661</v>
+      </c>
+      <c r="D81" t="s">
+        <v>655</v>
       </c>
       <c r="E81" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B82" t="s">
-        <v>739</v>
-      </c>
-      <c r="D82" t="s">
-        <v>740</v>
+        <v>671</v>
       </c>
       <c r="E82" t="s">
-        <v>741</v>
+        <v>670</v>
       </c>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B83" t="s">
-        <v>747</v>
-      </c>
-      <c r="C83" t="s">
-        <v>650</v>
+        <v>738</v>
       </c>
       <c r="D83" t="s">
-        <v>743</v>
+        <v>739</v>
+      </c>
+      <c r="E83" t="s">
+        <v>740</v>
       </c>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B84" s="5" t="s">
-        <v>673</v>
+      <c r="B84" t="s">
+        <v>746</v>
       </c>
       <c r="C84" t="s">
-        <v>664</v>
-      </c>
-      <c r="D84" s="5" t="s">
+        <v>649</v>
+      </c>
+      <c r="D84" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B85" s="5" t="s">
+        <v>672</v>
+      </c>
+      <c r="C85" t="s">
+        <v>663</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>679</v>
+      </c>
+      <c r="E85" s="5" t="s">
         <v>680</v>
-      </c>
-      <c r="E84" s="5" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B85" t="s">
-        <v>531</v>
-      </c>
-      <c r="C85" t="s">
-        <v>650</v>
-      </c>
-      <c r="D85" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B86" t="s">
-        <v>674</v>
+        <v>530</v>
+      </c>
+      <c r="C86" t="s">
+        <v>649</v>
       </c>
       <c r="D86" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B87" t="s">
-        <v>533</v>
-      </c>
-      <c r="C87" t="s">
-        <v>513</v>
+        <v>673</v>
       </c>
       <c r="D87" t="s">
-        <v>675</v>
-      </c>
-      <c r="E87" t="s">
-        <v>677</v>
+        <v>520</v>
       </c>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B88" t="s">
-        <v>748</v>
+        <v>532</v>
       </c>
       <c r="C88" t="s">
-        <v>650</v>
+        <v>513</v>
       </c>
       <c r="D88" t="s">
-        <v>743</v>
+        <v>674</v>
+      </c>
+      <c r="E88" t="s">
+        <v>676</v>
       </c>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B89" s="5" t="s">
-        <v>676</v>
+      <c r="B89" t="s">
+        <v>747</v>
       </c>
       <c r="C89" t="s">
-        <v>664</v>
-      </c>
-      <c r="D89" s="5" t="s">
+        <v>649</v>
+      </c>
+      <c r="D89" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B90" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="C90" t="s">
+        <v>663</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>679</v>
+      </c>
+      <c r="E90" s="5" t="s">
         <v>680</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B90" t="s">
-        <v>678</v>
-      </c>
-      <c r="C90" t="s">
-        <v>650</v>
-      </c>
-      <c r="D90" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B91" t="s">
-        <v>679</v>
+        <v>677</v>
+      </c>
+      <c r="C91" t="s">
+        <v>649</v>
       </c>
       <c r="D91" t="s">
-        <v>534</v>
-      </c>
-      <c r="E91" t="s">
-        <v>682</v>
+        <v>521</v>
       </c>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B92" t="s">
-        <v>684</v>
+        <v>678</v>
+      </c>
+      <c r="D92" t="s">
+        <v>533</v>
       </c>
       <c r="E92" t="s">
-        <v>558</v>
+        <v>681</v>
       </c>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B93" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="E93" t="s">
-        <v>683</v>
+        <v>557</v>
       </c>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B94" t="s">
-        <v>746</v>
-      </c>
-      <c r="C94" t="s">
-        <v>650</v>
-      </c>
-      <c r="D94" t="s">
-        <v>743</v>
+        <v>684</v>
+      </c>
+      <c r="E94" t="s">
+        <v>682</v>
       </c>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B95" s="5" t="s">
-        <v>686</v>
+      <c r="B95" t="s">
+        <v>745</v>
       </c>
       <c r="C95" t="s">
-        <v>664</v>
-      </c>
-      <c r="D95" s="5" t="s">
+        <v>649</v>
+      </c>
+      <c r="D95" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="96" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B96" s="5" t="s">
+        <v>685</v>
+      </c>
+      <c r="C96" t="s">
+        <v>663</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>679</v>
+      </c>
+      <c r="E96" s="5" t="s">
         <v>680</v>
-      </c>
-      <c r="E95" s="5" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B96" t="s">
-        <v>687</v>
-      </c>
-      <c r="C96" t="s">
-        <v>650</v>
-      </c>
-      <c r="D96" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B97" t="s">
+        <v>686</v>
+      </c>
+      <c r="C97" t="s">
+        <v>649</v>
+      </c>
+      <c r="D97" t="s">
         <v>705</v>
-      </c>
-      <c r="C97" t="s">
-        <v>513</v>
-      </c>
-      <c r="D97" t="s">
-        <v>707</v>
-      </c>
-      <c r="E97" t="s">
-        <v>708</v>
       </c>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B98" t="s">
         <v>704</v>
       </c>
+      <c r="C98" t="s">
+        <v>513</v>
+      </c>
+      <c r="D98" t="s">
+        <v>706</v>
+      </c>
       <c r="E98" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B99" t="s">
-        <v>712</v>
+        <v>703</v>
       </c>
       <c r="E99" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B100" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="E100" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
     </row>
     <row r="101" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B101" t="s">
-        <v>745</v>
-      </c>
-      <c r="C101" t="s">
-        <v>650</v>
-      </c>
-      <c r="D101" t="s">
-        <v>743</v>
+        <v>712</v>
+      </c>
+      <c r="E101" t="s">
+        <v>710</v>
       </c>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B102" s="5" t="s">
-        <v>714</v>
+      <c r="B102" t="s">
+        <v>744</v>
       </c>
       <c r="C102" t="s">
-        <v>664</v>
-      </c>
-      <c r="D102" s="5" t="s">
+        <v>649</v>
+      </c>
+      <c r="D102" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="103" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B103" s="5" t="s">
+        <v>713</v>
+      </c>
+      <c r="C103" t="s">
+        <v>663</v>
+      </c>
+      <c r="D103" s="5" t="s">
+        <v>679</v>
+      </c>
+      <c r="E103" s="5" t="s">
         <v>680</v>
-      </c>
-      <c r="E102" s="5" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B103" t="s">
-        <v>715</v>
-      </c>
-      <c r="C103" t="s">
-        <v>650</v>
-      </c>
-      <c r="D103" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B104" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="C104" t="s">
-        <v>718</v>
+        <v>649</v>
       </c>
       <c r="D104" t="s">
-        <v>689</v>
+        <v>534</v>
       </c>
     </row>
     <row r="105" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B105" t="s">
+        <v>715</v>
+      </c>
+      <c r="C105" t="s">
         <v>717</v>
       </c>
-      <c r="C105" t="s">
-        <v>719</v>
-      </c>
       <c r="D105" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="106" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B106" t="s">
+        <v>716</v>
+      </c>
+      <c r="C106" t="s">
+        <v>718</v>
+      </c>
+      <c r="D106" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B109" s="5" t="s">
+        <v>531</v>
+      </c>
+      <c r="C109" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="110" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B110" t="s">
         <v>695</v>
       </c>
-    </row>
-    <row r="108" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B108" s="5" t="s">
-        <v>532</v>
-      </c>
-      <c r="C108" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B109" t="s">
+      <c r="C110" t="s">
         <v>696</v>
-      </c>
-      <c r="C109" t="s">
-        <v>697</v>
       </c>
     </row>
   </sheetData>
@@ -25075,24 +25093,24 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>700</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>701</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="24" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B2" s="24"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="24" t="s">
+        <v>722</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>723</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>724</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
@@ -25103,33 +25121,33 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" s="24" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B6" s="24" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B7" s="24" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B8" s="24" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" s="24" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.4">
@@ -25141,7 +25159,7 @@
     <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" s="24"/>
       <c r="B11" s="24" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.4">
@@ -25154,17 +25172,17 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B14" s="24" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B15" s="24" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B16" s="24" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.4">
@@ -25172,25 +25190,25 @@
         <v>449</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B18" s="24" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B19" s="24" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A20" s="24" t="s">
+        <v>732</v>
+      </c>
+      <c r="B20" s="24" t="s">
         <v>733</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>734</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
0.0.b5 Change User Feedback from print to text box output
All necessary user feedbakc is put to the text box on the main screen. Will still need to do some cleanup of what this looks like, but on the whole this is functioning properly.
</commit_message>
<xml_diff>
--- a/Roadmap.xlsx
+++ b/Roadmap.xlsx
@@ -2312,10 +2312,10 @@
     <t>0.0.b44</t>
   </si>
   <si>
-    <t>Default TZ selection to Melbourne (already done)</t>
-  </si>
-  <si>
     <t>Fix multiple "Other" options in Timezone Region, also press ok without selecting location, only region</t>
+  </si>
+  <si>
+    <t>Default TZ selection to Melbourne</t>
   </si>
 </sst>
 </file>
@@ -23945,8 +23945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -24036,8 +24036,8 @@
       <c r="B6" t="s">
         <v>526</v>
       </c>
-      <c r="D6" t="s">
-        <v>758</v>
+      <c r="D6" s="24" t="s">
+        <v>759</v>
       </c>
       <c r="I6" t="s">
         <v>505</v>
@@ -24053,7 +24053,7 @@
       <c r="B7" t="s">
         <v>527</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="24" t="s">
         <v>524</v>
       </c>
       <c r="I7" t="s">
@@ -24448,7 +24448,7 @@
         <v>513</v>
       </c>
       <c r="D48" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
0.0.b12 Include Error Handling for empty GPS File
Error handling now implemented. If GPS Track file is empty file or cannot be read by Et module, throws an import error which is caught by the gui module. This then calls the "critical_error method which disables all buttons and advises / forces user to restart program.
</commit_message>
<xml_diff>
--- a/Roadmap.xlsx
+++ b/Roadmap.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="760">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="770">
   <si>
     <t>56 pixels</t>
   </si>
@@ -1712,9 +1712,6 @@
     <t>No track data in file</t>
   </si>
   <si>
-    <t>File too long</t>
-  </si>
-  <si>
     <t>Wrong Formatting</t>
   </si>
   <si>
@@ -2316,6 +2313,39 @@
   </si>
   <si>
     <t>Default TZ selection to Melbourne</t>
+  </si>
+  <si>
+    <t>0.0.b5.2</t>
+  </si>
+  <si>
+    <t>Test why index is out of range during full radar selection when creating kml</t>
+  </si>
+  <si>
+    <t>No internet coverage</t>
+  </si>
+  <si>
+    <t>0.0.b32.2</t>
+  </si>
+  <si>
+    <t>Solution</t>
+  </si>
+  <si>
+    <t>Errant files in the Radar filesystem. Introduced some file recognition statements</t>
+  </si>
+  <si>
+    <t>Already built in</t>
+  </si>
+  <si>
+    <t>Doesn't create as much of an error as expected.</t>
+  </si>
+  <si>
+    <t>No Issue</t>
+  </si>
+  <si>
+    <t>Implemented Error Handling, manually throw an ImportError, catch error, and use critical_error method to advise user and force restart</t>
+  </si>
+  <si>
+    <t>File too long (give user feedback)</t>
   </si>
 </sst>
 </file>
@@ -23943,10 +23973,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L110"/>
+  <dimension ref="A1:L112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -23954,6 +23984,7 @@
     <col min="3" max="3" width="25.921875" customWidth="1"/>
     <col min="4" max="4" width="56.3828125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.3828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.15234375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.4">
@@ -23972,6 +24003,9 @@
       <c r="E1" s="1" t="s">
         <v>551</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>763</v>
+      </c>
       <c r="I1" t="s">
         <v>494</v>
       </c>
@@ -24001,7 +24035,7 @@
         <v>513</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="I3" t="s">
         <v>497</v>
@@ -24012,7 +24046,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D4" s="24" t="s">
         <v>523</v>
@@ -24026,10 +24060,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.4">
@@ -24037,7 +24071,7 @@
         <v>526</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="I6" t="s">
         <v>505</v>
@@ -24068,9 +24102,9 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>586</v>
-      </c>
-      <c r="D8" t="s">
+        <v>585</v>
+      </c>
+      <c r="D8" s="24" t="s">
         <v>537</v>
       </c>
       <c r="I8" t="s">
@@ -24085,991 +24119,1022 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
-        <v>587</v>
-      </c>
-      <c r="D9" t="s">
-        <v>756</v>
+        <v>759</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>760</v>
+      </c>
+      <c r="F9" t="s">
+        <v>764</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
-        <v>588</v>
-      </c>
-      <c r="D10" t="s">
-        <v>539</v>
-      </c>
-      <c r="E10" t="s">
-        <v>552</v>
+        <v>586</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>755</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
-        <v>589</v>
-      </c>
-      <c r="D11" t="s">
-        <v>535</v>
-      </c>
-      <c r="E11" t="s">
-        <v>553</v>
+        <v>587</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>539</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>552</v>
+      </c>
+      <c r="F11" t="s">
+        <v>765</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
-        <v>590</v>
-      </c>
-      <c r="E12" t="s">
-        <v>554</v>
+        <v>588</v>
+      </c>
+      <c r="D12" t="s">
+        <v>535</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
-        <v>591</v>
-      </c>
-      <c r="E13" t="s">
-        <v>555</v>
+        <v>589</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
-        <v>592</v>
-      </c>
-      <c r="D14" t="s">
-        <v>536</v>
-      </c>
-      <c r="E14" t="s">
-        <v>556</v>
+        <v>590</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>555</v>
+      </c>
+      <c r="F14" t="s">
+        <v>766</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
-        <v>593</v>
-      </c>
-      <c r="E15" t="s">
-        <v>557</v>
+        <v>591</v>
+      </c>
+      <c r="D15" t="s">
+        <v>536</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>556</v>
+      </c>
+      <c r="F15" t="s">
+        <v>767</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
-        <v>594</v>
-      </c>
-      <c r="E16" t="s">
-        <v>558</v>
+        <v>592</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>557</v>
+      </c>
+      <c r="F16" t="s">
+        <v>768</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B17" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E17" t="s">
-        <v>751</v>
+        <v>769</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B18" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="E18" t="s">
-        <v>559</v>
+        <v>750</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B19" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="E19" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B20" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="E20" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
-        <v>599</v>
-      </c>
-      <c r="D21" t="s">
-        <v>538</v>
+        <v>597</v>
       </c>
       <c r="E21" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B22" t="s">
-        <v>600</v>
+        <v>598</v>
+      </c>
+      <c r="D22" t="s">
+        <v>538</v>
       </c>
       <c r="E22" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="E23" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
-        <v>602</v>
-      </c>
-      <c r="D24" t="s">
-        <v>541</v>
+        <v>600</v>
       </c>
       <c r="E24" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
-        <v>603</v>
+        <v>601</v>
+      </c>
+      <c r="D25" t="s">
+        <v>541</v>
       </c>
       <c r="E25" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B26" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="E26" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
-        <v>605</v>
-      </c>
-      <c r="D27" t="s">
-        <v>542</v>
+        <v>603</v>
       </c>
       <c r="E27" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
-        <v>606</v>
+        <v>604</v>
+      </c>
+      <c r="D28" t="s">
+        <v>542</v>
       </c>
       <c r="E28" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="E29" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
-        <v>608</v>
-      </c>
-      <c r="D30" t="s">
-        <v>543</v>
+        <v>606</v>
       </c>
       <c r="E30" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B31" t="s">
-        <v>609</v>
+        <v>607</v>
+      </c>
+      <c r="D31" t="s">
+        <v>543</v>
       </c>
       <c r="E31" t="s">
-        <v>569</v>
+        <v>573</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="E32" t="s">
-        <v>575</v>
+        <v>568</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="E33" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B34" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="E34" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B35" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="E35" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B36" t="s">
-        <v>614</v>
-      </c>
-      <c r="D36" t="s">
-        <v>544</v>
+        <v>612</v>
       </c>
       <c r="E36" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B37" t="s">
-        <v>615</v>
-      </c>
-      <c r="D37" t="s">
-        <v>545</v>
+        <v>762</v>
       </c>
       <c r="E37" t="s">
-        <v>580</v>
+        <v>761</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
-        <v>616</v>
+        <v>613</v>
+      </c>
+      <c r="D38" t="s">
+        <v>544</v>
       </c>
       <c r="E38" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B39" t="s">
-        <v>617</v>
+        <v>614</v>
+      </c>
+      <c r="D39" t="s">
+        <v>545</v>
       </c>
       <c r="E39" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B40" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="E40" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B41" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="E41" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B42" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="E42" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B43" t="s">
-        <v>621</v>
-      </c>
-      <c r="D43" t="s">
-        <v>549</v>
+        <v>618</v>
       </c>
       <c r="E43" t="s">
-        <v>579</v>
+        <v>583</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B44" t="s">
-        <v>752</v>
-      </c>
-      <c r="D44" t="s">
-        <v>753</v>
+        <v>619</v>
       </c>
       <c r="E44" t="s">
-        <v>754</v>
+        <v>584</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B45" t="s">
-        <v>691</v>
-      </c>
-      <c r="C45" t="s">
-        <v>649</v>
+        <v>620</v>
       </c>
       <c r="D45" t="s">
-        <v>689</v>
+        <v>549</v>
+      </c>
+      <c r="E45" t="s">
+        <v>578</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B46" t="s">
-        <v>690</v>
-      </c>
-      <c r="C46" t="s">
-        <v>513</v>
+        <v>751</v>
       </c>
       <c r="D46" t="s">
-        <v>693</v>
+        <v>752</v>
       </c>
       <c r="E46" t="s">
-        <v>692</v>
+        <v>753</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B47" t="s">
-        <v>741</v>
+        <v>690</v>
       </c>
       <c r="C47" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D47" t="s">
-        <v>742</v>
+        <v>688</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B48" t="s">
-        <v>757</v>
+        <v>689</v>
       </c>
       <c r="C48" t="s">
         <v>513</v>
       </c>
       <c r="D48" t="s">
-        <v>758</v>
+        <v>692</v>
+      </c>
+      <c r="E48" t="s">
+        <v>691</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B49" s="5" t="s">
-        <v>662</v>
+      <c r="B49" t="s">
+        <v>740</v>
       </c>
       <c r="C49" t="s">
-        <v>663</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>679</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>680</v>
+        <v>648</v>
+      </c>
+      <c r="D49" t="s">
+        <v>741</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B50" t="s">
-        <v>514</v>
+        <v>756</v>
       </c>
       <c r="C50" t="s">
-        <v>649</v>
+        <v>513</v>
       </c>
       <c r="D50" t="s">
-        <v>515</v>
+        <v>757</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B51" t="s">
-        <v>629</v>
+      <c r="B51" s="5" t="s">
+        <v>661</v>
       </c>
       <c r="C51" t="s">
-        <v>513</v>
-      </c>
-      <c r="D51" t="s">
-        <v>623</v>
-      </c>
-      <c r="E51" t="s">
-        <v>624</v>
+        <v>662</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>678</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>679</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B52" t="s">
-        <v>630</v>
-      </c>
-      <c r="E52" t="s">
-        <v>625</v>
+        <v>514</v>
+      </c>
+      <c r="C52" t="s">
+        <v>648</v>
+      </c>
+      <c r="D52" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B53" t="s">
-        <v>631</v>
+        <v>628</v>
+      </c>
+      <c r="C53" t="s">
+        <v>513</v>
+      </c>
+      <c r="D53" t="s">
+        <v>622</v>
       </c>
       <c r="E53" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B54" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="E54" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B55" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="E55" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B56" t="s">
-        <v>743</v>
-      </c>
-      <c r="C56" t="s">
-        <v>649</v>
-      </c>
-      <c r="D56" t="s">
-        <v>742</v>
+        <v>631</v>
+      </c>
+      <c r="E56" t="s">
+        <v>626</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B57" s="5" t="s">
-        <v>664</v>
-      </c>
-      <c r="C57" t="s">
-        <v>663</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>679</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>680</v>
+      <c r="B57" t="s">
+        <v>632</v>
+      </c>
+      <c r="E57" t="s">
+        <v>627</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B58" t="s">
-        <v>525</v>
+        <v>742</v>
       </c>
       <c r="C58" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D58" t="s">
-        <v>516</v>
+        <v>741</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B59" t="s">
-        <v>528</v>
-      </c>
-      <c r="D59" t="s">
-        <v>518</v>
+      <c r="B59" s="5" t="s">
+        <v>663</v>
+      </c>
+      <c r="C59" t="s">
+        <v>662</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>678</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>679</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B60" t="s">
-        <v>565</v>
+        <v>525</v>
+      </c>
+      <c r="C60" t="s">
+        <v>648</v>
       </c>
       <c r="D60" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B61" t="s">
-        <v>566</v>
+        <v>528</v>
       </c>
       <c r="D61" t="s">
-        <v>540</v>
+        <v>518</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B62" t="s">
-        <v>749</v>
+        <v>564</v>
       </c>
       <c r="D62" t="s">
-        <v>750</v>
+        <v>522</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B63" t="s">
-        <v>643</v>
-      </c>
-      <c r="C63" t="s">
-        <v>513</v>
+        <v>565</v>
       </c>
       <c r="D63" t="s">
-        <v>634</v>
-      </c>
-      <c r="E63" t="s">
-        <v>638</v>
+        <v>540</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B64" t="s">
-        <v>644</v>
-      </c>
-      <c r="E64" t="s">
-        <v>639</v>
+        <v>748</v>
+      </c>
+      <c r="D64" t="s">
+        <v>749</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B65" t="s">
-        <v>645</v>
+        <v>642</v>
+      </c>
+      <c r="C65" t="s">
+        <v>513</v>
       </c>
       <c r="D65" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="E65" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B66" t="s">
-        <v>646</v>
-      </c>
-      <c r="D66" t="s">
-        <v>636</v>
+        <v>643</v>
       </c>
       <c r="E66" t="s">
-        <v>111</v>
+        <v>638</v>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B67" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="D67" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="E67" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B68" t="s">
-        <v>648</v>
+        <v>645</v>
+      </c>
+      <c r="D68" t="s">
+        <v>635</v>
       </c>
       <c r="E68" t="s">
-        <v>642</v>
+        <v>111</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B69" t="s">
-        <v>748</v>
-      </c>
-      <c r="C69" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="D69" t="s">
-        <v>742</v>
+        <v>636</v>
+      </c>
+      <c r="E69" t="s">
+        <v>640</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B70" s="5" t="s">
-        <v>665</v>
-      </c>
-      <c r="C70" t="s">
-        <v>663</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>679</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>680</v>
+      <c r="B70" t="s">
+        <v>647</v>
+      </c>
+      <c r="E70" t="s">
+        <v>641</v>
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B71" t="s">
-        <v>529</v>
+        <v>747</v>
       </c>
       <c r="C71" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D71" t="s">
-        <v>546</v>
+        <v>741</v>
       </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B72" t="s">
-        <v>567</v>
-      </c>
-      <c r="D72" t="s">
-        <v>517</v>
+      <c r="B72" s="5" t="s">
+        <v>664</v>
+      </c>
+      <c r="C72" t="s">
+        <v>662</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>678</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>679</v>
       </c>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B73" t="s">
-        <v>650</v>
+        <v>529</v>
+      </c>
+      <c r="C73" t="s">
+        <v>648</v>
       </c>
       <c r="D73" t="s">
-        <v>654</v>
+        <v>546</v>
       </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B74" t="s">
-        <v>651</v>
+        <v>566</v>
       </c>
       <c r="D74" t="s">
-        <v>564</v>
+        <v>517</v>
       </c>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B75" t="s">
-        <v>736</v>
+        <v>649</v>
       </c>
       <c r="D75" t="s">
-        <v>737</v>
+        <v>653</v>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B76" t="s">
-        <v>547</v>
-      </c>
-      <c r="C76" t="s">
-        <v>513</v>
+        <v>650</v>
       </c>
       <c r="D76" t="s">
-        <v>652</v>
-      </c>
-      <c r="E76" t="s">
-        <v>656</v>
+        <v>563</v>
       </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B77" t="s">
-        <v>548</v>
-      </c>
-      <c r="E77" t="s">
-        <v>657</v>
+        <v>735</v>
+      </c>
+      <c r="D77" t="s">
+        <v>736</v>
       </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B78" t="s">
-        <v>658</v>
+        <v>547</v>
+      </c>
+      <c r="C78" t="s">
+        <v>513</v>
       </c>
       <c r="D78" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="E78" t="s">
-        <v>666</v>
+        <v>655</v>
       </c>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B79" t="s">
-        <v>659</v>
+        <v>548</v>
       </c>
       <c r="E79" t="s">
-        <v>667</v>
+        <v>656</v>
       </c>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B80" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="D80" t="s">
-        <v>668</v>
+        <v>652</v>
       </c>
       <c r="E80" t="s">
-        <v>111</v>
+        <v>665</v>
       </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B81" t="s">
-        <v>661</v>
-      </c>
-      <c r="D81" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
       <c r="E81" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B82" t="s">
-        <v>671</v>
+        <v>659</v>
+      </c>
+      <c r="D82" t="s">
+        <v>667</v>
       </c>
       <c r="E82" t="s">
-        <v>670</v>
+        <v>111</v>
       </c>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B83" t="s">
-        <v>738</v>
+        <v>660</v>
       </c>
       <c r="D83" t="s">
-        <v>739</v>
+        <v>654</v>
       </c>
       <c r="E83" t="s">
-        <v>740</v>
+        <v>668</v>
       </c>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B84" t="s">
-        <v>746</v>
-      </c>
-      <c r="C84" t="s">
-        <v>649</v>
-      </c>
-      <c r="D84" t="s">
-        <v>742</v>
+        <v>670</v>
+      </c>
+      <c r="E84" t="s">
+        <v>669</v>
       </c>
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B85" s="5" t="s">
-        <v>672</v>
-      </c>
-      <c r="C85" t="s">
-        <v>663</v>
-      </c>
-      <c r="D85" s="5" t="s">
-        <v>679</v>
-      </c>
-      <c r="E85" s="5" t="s">
-        <v>680</v>
+      <c r="B85" t="s">
+        <v>737</v>
+      </c>
+      <c r="D85" t="s">
+        <v>738</v>
+      </c>
+      <c r="E85" t="s">
+        <v>739</v>
       </c>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B86" t="s">
-        <v>530</v>
+        <v>745</v>
       </c>
       <c r="C86" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D86" t="s">
-        <v>519</v>
+        <v>741</v>
       </c>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B87" t="s">
-        <v>673</v>
-      </c>
-      <c r="D87" t="s">
-        <v>520</v>
+      <c r="B87" s="5" t="s">
+        <v>671</v>
+      </c>
+      <c r="C87" t="s">
+        <v>662</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>678</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>679</v>
       </c>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B88" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C88" t="s">
-        <v>513</v>
+        <v>648</v>
       </c>
       <c r="D88" t="s">
-        <v>674</v>
-      </c>
-      <c r="E88" t="s">
-        <v>676</v>
+        <v>519</v>
       </c>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B89" t="s">
-        <v>747</v>
-      </c>
-      <c r="C89" t="s">
-        <v>649</v>
+        <v>672</v>
       </c>
       <c r="D89" t="s">
-        <v>742</v>
+        <v>520</v>
       </c>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B90" s="5" t="s">
+      <c r="B90" t="s">
+        <v>532</v>
+      </c>
+      <c r="C90" t="s">
+        <v>513</v>
+      </c>
+      <c r="D90" t="s">
+        <v>673</v>
+      </c>
+      <c r="E90" t="s">
         <v>675</v>
-      </c>
-      <c r="C90" t="s">
-        <v>663</v>
-      </c>
-      <c r="D90" s="5" t="s">
-        <v>679</v>
-      </c>
-      <c r="E90" s="5" t="s">
-        <v>680</v>
       </c>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B91" t="s">
-        <v>677</v>
+        <v>746</v>
       </c>
       <c r="C91" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D91" t="s">
-        <v>521</v>
+        <v>741</v>
       </c>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B92" t="s">
+      <c r="B92" s="5" t="s">
+        <v>674</v>
+      </c>
+      <c r="C92" t="s">
+        <v>662</v>
+      </c>
+      <c r="D92" s="5" t="s">
         <v>678</v>
       </c>
-      <c r="D92" t="s">
-        <v>533</v>
-      </c>
-      <c r="E92" t="s">
-        <v>681</v>
+      <c r="E92" s="5" t="s">
+        <v>679</v>
       </c>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B93" t="s">
-        <v>683</v>
-      </c>
-      <c r="E93" t="s">
-        <v>557</v>
+        <v>676</v>
+      </c>
+      <c r="C93" t="s">
+        <v>648</v>
+      </c>
+      <c r="D93" t="s">
+        <v>521</v>
       </c>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B94" t="s">
-        <v>684</v>
+        <v>677</v>
+      </c>
+      <c r="D94" t="s">
+        <v>533</v>
       </c>
       <c r="E94" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B95" t="s">
-        <v>745</v>
-      </c>
-      <c r="C95" t="s">
-        <v>649</v>
-      </c>
-      <c r="D95" t="s">
-        <v>742</v>
+        <v>682</v>
+      </c>
+      <c r="E95" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B96" s="5" t="s">
-        <v>685</v>
-      </c>
-      <c r="C96" t="s">
-        <v>663</v>
-      </c>
-      <c r="D96" s="5" t="s">
-        <v>679</v>
-      </c>
-      <c r="E96" s="5" t="s">
-        <v>680</v>
+      <c r="B96" t="s">
+        <v>683</v>
+      </c>
+      <c r="E96" t="s">
+        <v>681</v>
       </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B97" t="s">
-        <v>686</v>
+        <v>744</v>
       </c>
       <c r="C97" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D97" t="s">
-        <v>705</v>
+        <v>741</v>
       </c>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B98" t="s">
-        <v>704</v>
+      <c r="B98" s="5" t="s">
+        <v>684</v>
       </c>
       <c r="C98" t="s">
-        <v>513</v>
-      </c>
-      <c r="D98" t="s">
-        <v>706</v>
-      </c>
-      <c r="E98" t="s">
-        <v>707</v>
+        <v>662</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>678</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>679</v>
       </c>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B99" t="s">
-        <v>703</v>
-      </c>
-      <c r="E99" t="s">
-        <v>708</v>
+        <v>685</v>
+      </c>
+      <c r="C99" t="s">
+        <v>648</v>
+      </c>
+      <c r="D99" t="s">
+        <v>704</v>
       </c>
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B100" t="s">
-        <v>711</v>
+        <v>703</v>
+      </c>
+      <c r="C100" t="s">
+        <v>513</v>
+      </c>
+      <c r="D100" t="s">
+        <v>705</v>
       </c>
       <c r="E100" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
     </row>
     <row r="101" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B101" t="s">
-        <v>712</v>
+        <v>702</v>
       </c>
       <c r="E101" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B102" t="s">
-        <v>744</v>
-      </c>
-      <c r="C102" t="s">
-        <v>649</v>
-      </c>
-      <c r="D102" t="s">
-        <v>742</v>
+        <v>710</v>
+      </c>
+      <c r="E102" t="s">
+        <v>708</v>
       </c>
     </row>
     <row r="103" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B103" s="5" t="s">
-        <v>713</v>
-      </c>
-      <c r="C103" t="s">
-        <v>663</v>
-      </c>
-      <c r="D103" s="5" t="s">
-        <v>679</v>
-      </c>
-      <c r="E103" s="5" t="s">
-        <v>680</v>
+      <c r="B103" t="s">
+        <v>711</v>
+      </c>
+      <c r="E103" t="s">
+        <v>709</v>
       </c>
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B104" t="s">
-        <v>714</v>
+        <v>743</v>
       </c>
       <c r="C104" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D104" t="s">
-        <v>534</v>
+        <v>741</v>
       </c>
     </row>
     <row r="105" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B105" t="s">
-        <v>715</v>
+      <c r="B105" s="5" t="s">
+        <v>712</v>
       </c>
       <c r="C105" t="s">
-        <v>717</v>
-      </c>
-      <c r="D105" t="s">
-        <v>688</v>
+        <v>662</v>
+      </c>
+      <c r="D105" s="5" t="s">
+        <v>678</v>
+      </c>
+      <c r="E105" s="5" t="s">
+        <v>679</v>
       </c>
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B106" t="s">
+        <v>713</v>
+      </c>
+      <c r="C106" t="s">
+        <v>648</v>
+      </c>
+      <c r="D106" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B107" t="s">
+        <v>714</v>
+      </c>
+      <c r="C107" t="s">
         <v>716</v>
       </c>
-      <c r="C106" t="s">
-        <v>718</v>
-      </c>
-      <c r="D106" t="s">
+      <c r="D107" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B108" t="s">
+        <v>715</v>
+      </c>
+      <c r="C108" t="s">
+        <v>717</v>
+      </c>
+      <c r="D108" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="111" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B111" s="5" t="s">
+        <v>531</v>
+      </c>
+      <c r="C111" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="112" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B112" t="s">
         <v>694</v>
       </c>
-    </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B109" s="5" t="s">
-        <v>531</v>
-      </c>
-      <c r="C109" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="110" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B110" t="s">
+      <c r="C112" t="s">
         <v>695</v>
-      </c>
-      <c r="C110" t="s">
-        <v>696</v>
       </c>
     </row>
   </sheetData>
@@ -25093,24 +25158,24 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>699</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="24" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B2" s="24"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="24" t="s">
+        <v>721</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>722</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>723</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
@@ -25121,33 +25186,33 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" s="24" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B6" s="24" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B7" s="24" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B8" s="24" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" s="24" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.4">
@@ -25159,7 +25224,7 @@
     <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" s="24"/>
       <c r="B11" s="24" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.4">
@@ -25172,17 +25237,17 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B14" s="24" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B15" s="24" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B16" s="24" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.4">
@@ -25190,25 +25255,25 @@
         <v>449</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B18" s="24" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B19" s="24" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A20" s="24" t="s">
+        <v>731</v>
+      </c>
+      <c r="B20" s="24" t="s">
         <v>732</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>733</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
0.0.b14 Error Handling for Short GPS Files
Error handling for files that have less than 2 GPS points now implemented. Also cleaned up some other areas of code that were giving bad results for small files.
</commit_message>
<xml_diff>
--- a/Roadmap.xlsx
+++ b/Roadmap.xlsx
@@ -15,16 +15,16 @@
     <sheet name="Roadmap" sheetId="2" r:id="rId1"/>
     <sheet name="Versioning" sheetId="15" r:id="rId2"/>
     <sheet name="Documentation" sheetId="16" r:id="rId3"/>
-    <sheet name="Redesign" sheetId="11" r:id="rId4"/>
-    <sheet name="GUI Design" sheetId="13" r:id="rId5"/>
-    <sheet name="Time Testing" sheetId="12" r:id="rId6"/>
-    <sheet name="Design" sheetId="10" r:id="rId7"/>
-    <sheet name="Initial Inputs" sheetId="8" r:id="rId8"/>
-    <sheet name="Radar Sites" sheetId="7" r:id="rId9"/>
-    <sheet name="KML Radar Construct" sheetId="4" r:id="rId10"/>
-    <sheet name="Workings" sheetId="1" r:id="rId11"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId12"/>
-    <sheet name="Sheet2" sheetId="9" r:id="rId13"/>
+    <sheet name="Code Stats Summary" sheetId="9" r:id="rId4"/>
+    <sheet name="Redesign" sheetId="11" r:id="rId5"/>
+    <sheet name="GUI Design" sheetId="13" r:id="rId6"/>
+    <sheet name="Time Testing" sheetId="12" r:id="rId7"/>
+    <sheet name="Design" sheetId="10" r:id="rId8"/>
+    <sheet name="Initial Inputs" sheetId="8" r:id="rId9"/>
+    <sheet name="Radar Sites" sheetId="7" r:id="rId10"/>
+    <sheet name="KML Radar Construct" sheetId="4" r:id="rId11"/>
+    <sheet name="Workings" sheetId="1" r:id="rId12"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId13"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="770">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="781">
   <si>
     <t>56 pixels</t>
   </si>
@@ -2346,6 +2346,39 @@
   </si>
   <si>
     <t>File too long (give user feedback)</t>
+  </si>
+  <si>
+    <t>main</t>
+  </si>
+  <si>
+    <t>icondata</t>
+  </si>
+  <si>
+    <t>kml creator</t>
+  </si>
+  <si>
+    <t>radar methods</t>
+  </si>
+  <si>
+    <t>radar overlays</t>
+  </si>
+  <si>
+    <t>timezones</t>
+  </si>
+  <si>
+    <t>media methods</t>
+  </si>
+  <si>
+    <t>radar download frames</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Total Code</t>
+  </si>
+  <si>
+    <t>User Code (Not Auto Generated)</t>
   </si>
 </sst>
 </file>
@@ -2892,7 +2925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -3165,6 +3198,631 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="6" customWidth="1"/>
+    <col min="2" max="2" width="4.4609375" customWidth="1"/>
+    <col min="3" max="4" width="2.84375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.84375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.4609375" customWidth="1"/>
+    <col min="7" max="8" width="2.84375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.23046875" customWidth="1"/>
+    <col min="11" max="12" width="2.84375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.921875" customWidth="1"/>
+    <col min="15" max="16" width="2.84375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.84375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4">
+        <v>37</v>
+      </c>
+      <c r="C4">
+        <v>17</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <f>B4+(C4/60)+(D4/(60*60))</f>
+        <v>37.284444444444439</v>
+      </c>
+      <c r="F4">
+        <v>35</v>
+      </c>
+      <c r="G4">
+        <v>42</v>
+      </c>
+      <c r="H4">
+        <v>32</v>
+      </c>
+      <c r="I4">
+        <f>F4+(G4/60)+(H4/(60*60))</f>
+        <v>35.708888888888893</v>
+      </c>
+      <c r="J4">
+        <v>35</v>
+      </c>
+      <c r="K4">
+        <v>33</v>
+      </c>
+      <c r="L4">
+        <v>28</v>
+      </c>
+      <c r="M4">
+        <f>J4+(K4/60)+(L4/(60*60))</f>
+        <v>35.557777777777773</v>
+      </c>
+      <c r="N4">
+        <v>33</v>
+      </c>
+      <c r="O4">
+        <v>15</v>
+      </c>
+      <c r="P4">
+        <v>20</v>
+      </c>
+      <c r="Q4">
+        <f>N4+(O4/60)+(P4/(60*60))</f>
+        <v>33.255555555555553</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5">
+        <v>145</v>
+      </c>
+      <c r="C5">
+        <v>29</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <f>B5+(C5/60)+(D5/(60*60))</f>
+        <v>145.48888888888888</v>
+      </c>
+      <c r="F5">
+        <v>146</v>
+      </c>
+      <c r="G5">
+        <v>13</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <f>F5+(G5/60)+(H5/(60*60))</f>
+        <v>146.21777777777777</v>
+      </c>
+      <c r="J5">
+        <v>147</v>
+      </c>
+      <c r="K5">
+        <v>40</v>
+      </c>
+      <c r="L5">
+        <v>30</v>
+      </c>
+      <c r="M5">
+        <f>J5+(K5/60)+(L5/(60*60))</f>
+        <v>147.67499999999998</v>
+      </c>
+      <c r="N5">
+        <v>150</v>
+      </c>
+      <c r="O5">
+        <v>35</v>
+      </c>
+      <c r="P5">
+        <v>4</v>
+      </c>
+      <c r="Q5">
+        <f>N5+(O5/60)+(P5/(60*60))</f>
+        <v>150.58444444444444</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6">
+        <v>38</v>
+      </c>
+      <c r="C6">
+        <v>26</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <f>B6+(C6/60)+(D6/(60*60))</f>
+        <v>38.435555555555553</v>
+      </c>
+      <c r="F6">
+        <v>39</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>40</v>
+      </c>
+      <c r="I6">
+        <f>F6+(G6/60)+(H6/(60*60))</f>
+        <v>39.011111111111113</v>
+      </c>
+      <c r="J6">
+        <v>40</v>
+      </c>
+      <c r="K6">
+        <v>9</v>
+      </c>
+      <c r="L6">
+        <v>44</v>
+      </c>
+      <c r="M6">
+        <f>J6+(K6/60)+(L6/(60*60))</f>
+        <v>40.162222222222219</v>
+      </c>
+      <c r="N6">
+        <v>42</v>
+      </c>
+      <c r="O6">
+        <v>27</v>
+      </c>
+      <c r="P6">
+        <v>52</v>
+      </c>
+      <c r="Q6">
+        <f>N6+(O6/60)+(P6/(60*60))</f>
+        <v>42.464444444444446</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7">
+        <v>144</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>52</v>
+      </c>
+      <c r="E7">
+        <f>B7+(C7/60)+(D7/(60*60))</f>
+        <v>144.03111111111113</v>
+      </c>
+      <c r="F7">
+        <v>143</v>
+      </c>
+      <c r="G7">
+        <v>18</v>
+      </c>
+      <c r="H7">
+        <v>8</v>
+      </c>
+      <c r="I7">
+        <f>F7+(G7/60)+(H7/(60*60))</f>
+        <v>143.30222222222224</v>
+      </c>
+      <c r="J7">
+        <v>141</v>
+      </c>
+      <c r="K7">
+        <v>50</v>
+      </c>
+      <c r="L7">
+        <v>42</v>
+      </c>
+      <c r="M7">
+        <f>J7+(K7/60)+(L7/(60*60))</f>
+        <v>141.845</v>
+      </c>
+      <c r="N7">
+        <v>138</v>
+      </c>
+      <c r="O7">
+        <v>56</v>
+      </c>
+      <c r="P7">
+        <v>8</v>
+      </c>
+      <c r="Q7">
+        <f>N7+(O7/60)+(P7/(60*60))</f>
+        <v>138.93555555555557</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A9" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" t="s">
+        <v>3</v>
+      </c>
+      <c r="L11" t="s">
+        <v>4</v>
+      </c>
+      <c r="M11" t="s">
+        <v>5</v>
+      </c>
+      <c r="N11" t="s">
+        <v>2</v>
+      </c>
+      <c r="O11" t="s">
+        <v>3</v>
+      </c>
+      <c r="P11" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12">
+        <v>35</v>
+      </c>
+      <c r="C12">
+        <v>27</v>
+      </c>
+      <c r="D12">
+        <v>16</v>
+      </c>
+      <c r="E12">
+        <f>B12+(C12/60)+(D12/(60*60))</f>
+        <v>35.454444444444448</v>
+      </c>
+      <c r="F12">
+        <v>34</v>
+      </c>
+      <c r="G12">
+        <v>52</v>
+      </c>
+      <c r="H12">
+        <v>44</v>
+      </c>
+      <c r="I12">
+        <f>F12+(G12/60)+(H12/(60*60))</f>
+        <v>34.878888888888888</v>
+      </c>
+      <c r="J12">
+        <v>33</v>
+      </c>
+      <c r="K12">
+        <v>43</v>
+      </c>
+      <c r="L12">
+        <v>40</v>
+      </c>
+      <c r="M12">
+        <f>J12+(K12/60)+(L12/(60*60))</f>
+        <v>33.727777777777781</v>
+      </c>
+      <c r="N12">
+        <v>31</v>
+      </c>
+      <c r="O12">
+        <v>25</v>
+      </c>
+      <c r="P12">
+        <v>32</v>
+      </c>
+      <c r="Q12">
+        <f>N12+(O12/60)+(P12/(60*60))</f>
+        <v>31.425555555555558</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13">
+        <v>146</v>
+      </c>
+      <c r="C13">
+        <v>44</v>
+      </c>
+      <c r="D13">
+        <v>30</v>
+      </c>
+      <c r="E13">
+        <f>B13+(C13/60)+(D13/(60*60))</f>
+        <v>146.74166666666665</v>
+      </c>
+      <c r="F13">
+        <v>147</v>
+      </c>
+      <c r="G13">
+        <v>27</v>
+      </c>
+      <c r="H13">
+        <v>12</v>
+      </c>
+      <c r="I13">
+        <f>F13+(G13/60)+(H13/(60*60))</f>
+        <v>147.45333333333332</v>
+      </c>
+      <c r="J13">
+        <v>148</v>
+      </c>
+      <c r="K13">
+        <v>52</v>
+      </c>
+      <c r="L13">
+        <v>34</v>
+      </c>
+      <c r="M13">
+        <f>J13+(K13/60)+(L13/(60*60))</f>
+        <v>148.87611111111113</v>
+      </c>
+      <c r="N13">
+        <v>151</v>
+      </c>
+      <c r="O13">
+        <v>43</v>
+      </c>
+      <c r="P13">
+        <v>2</v>
+      </c>
+      <c r="Q13">
+        <f>N13+(O13/60)+(P13/(60*60))</f>
+        <v>151.71722222222223</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14">
+        <v>36</v>
+      </c>
+      <c r="C14">
+        <v>36</v>
+      </c>
+      <c r="D14">
+        <v>20</v>
+      </c>
+      <c r="E14">
+        <f>B14+(C14/60)+(D14/(60*60))</f>
+        <v>36.605555555555554</v>
+      </c>
+      <c r="F14">
+        <v>37</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>52</v>
+      </c>
+      <c r="I14">
+        <f>F14+(G14/60)+(H14/(60*60))</f>
+        <v>37.181111111111107</v>
+      </c>
+      <c r="J14">
+        <v>38</v>
+      </c>
+      <c r="K14">
+        <v>19</v>
+      </c>
+      <c r="L14">
+        <v>56</v>
+      </c>
+      <c r="M14">
+        <f>J14+(K14/60)+(L14/(60*60))</f>
+        <v>38.332222222222228</v>
+      </c>
+      <c r="N14">
+        <v>40</v>
+      </c>
+      <c r="O14">
+        <v>38</v>
+      </c>
+      <c r="P14">
+        <v>4</v>
+      </c>
+      <c r="Q14">
+        <f>N14+(O14/60)+(P14/(60*60))</f>
+        <v>40.634444444444441</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15">
+        <v>145</v>
+      </c>
+      <c r="C15">
+        <v>19</v>
+      </c>
+      <c r="D15">
+        <v>6</v>
+      </c>
+      <c r="E15">
+        <f>B15+(C15/60)+(D15/(60*60))</f>
+        <v>145.31833333333333</v>
+      </c>
+      <c r="F15">
+        <v>144</v>
+      </c>
+      <c r="G15">
+        <v>36</v>
+      </c>
+      <c r="H15">
+        <v>24</v>
+      </c>
+      <c r="I15">
+        <f>F15+(G15/60)+(H15/(60*60))</f>
+        <v>144.60666666666665</v>
+      </c>
+      <c r="J15">
+        <v>143</v>
+      </c>
+      <c r="K15">
+        <v>11</v>
+      </c>
+      <c r="L15">
+        <v>22</v>
+      </c>
+      <c r="M15">
+        <f>J15+(K15/60)+(L15/(60*60))</f>
+        <v>143.18944444444446</v>
+      </c>
+      <c r="N15">
+        <v>140</v>
+      </c>
+      <c r="O15">
+        <v>20</v>
+      </c>
+      <c r="P15">
+        <v>34</v>
+      </c>
+      <c r="Q15">
+        <f>N15+(O15/60)+(P15/(60*60))</f>
+        <v>140.3427777777778</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2708"/>
   <sheetViews>
@@ -23771,7 +24429,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O16"/>
   <sheetViews>
@@ -23898,7 +24556,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -23953,20 +24611,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -24154,7 +24798,7 @@
       <c r="B12" t="s">
         <v>588</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="24" t="s">
         <v>535</v>
       </c>
       <c r="E12" s="24" t="s">
@@ -24209,7 +24853,7 @@
       <c r="B17" t="s">
         <v>593</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="24" t="s">
         <v>769</v>
       </c>
     </row>
@@ -25284,9 +25928,142 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="13.15234375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>770</v>
+      </c>
+      <c r="B1">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>339</v>
+      </c>
+      <c r="B2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>325</v>
+      </c>
+      <c r="B3">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>771</v>
+      </c>
+      <c r="B4">
+        <v>219</v>
+      </c>
+      <c r="C4" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>772</v>
+      </c>
+      <c r="B5">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>773</v>
+      </c>
+      <c r="B6">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>774</v>
+      </c>
+      <c r="B7">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>775</v>
+      </c>
+      <c r="B8">
+        <v>607</v>
+      </c>
+      <c r="C8" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>776</v>
+      </c>
+      <c r="B9">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>327</v>
+      </c>
+      <c r="B10">
+        <v>613</v>
+      </c>
+      <c r="C10" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>777</v>
+      </c>
+      <c r="B11">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B12" t="s">
+        <v>779</v>
+      </c>
+      <c r="C12" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B13">
+        <f>SUM(B1:B11)</f>
+        <v>3899</v>
+      </c>
+      <c r="C13">
+        <f>SUM(B1:B11)-B10-B8-B4</f>
+        <v>2460</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F109"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A134" workbookViewId="0">
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
@@ -25875,7 +26652,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K36"/>
   <sheetViews>
@@ -26147,7 +26924,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:M14"/>
   <sheetViews>
@@ -26467,7 +27244,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -27659,7 +28436,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D19"/>
   <sheetViews>
@@ -27752,629 +28529,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="4.4609375" customWidth="1"/>
-    <col min="3" max="4" width="2.84375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.84375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.4609375" customWidth="1"/>
-    <col min="7" max="8" width="2.84375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.84375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.23046875" customWidth="1"/>
-    <col min="11" max="12" width="2.84375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.921875" customWidth="1"/>
-    <col min="15" max="16" width="2.84375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.84375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" t="s">
-        <v>3</v>
-      </c>
-      <c r="L3" t="s">
-        <v>4</v>
-      </c>
-      <c r="M3" t="s">
-        <v>5</v>
-      </c>
-      <c r="N3" t="s">
-        <v>2</v>
-      </c>
-      <c r="O3" t="s">
-        <v>3</v>
-      </c>
-      <c r="P3" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4">
-        <v>37</v>
-      </c>
-      <c r="C4">
-        <v>17</v>
-      </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-      <c r="E4">
-        <f>B4+(C4/60)+(D4/(60*60))</f>
-        <v>37.284444444444439</v>
-      </c>
-      <c r="F4">
-        <v>35</v>
-      </c>
-      <c r="G4">
-        <v>42</v>
-      </c>
-      <c r="H4">
-        <v>32</v>
-      </c>
-      <c r="I4">
-        <f>F4+(G4/60)+(H4/(60*60))</f>
-        <v>35.708888888888893</v>
-      </c>
-      <c r="J4">
-        <v>35</v>
-      </c>
-      <c r="K4">
-        <v>33</v>
-      </c>
-      <c r="L4">
-        <v>28</v>
-      </c>
-      <c r="M4">
-        <f>J4+(K4/60)+(L4/(60*60))</f>
-        <v>35.557777777777773</v>
-      </c>
-      <c r="N4">
-        <v>33</v>
-      </c>
-      <c r="O4">
-        <v>15</v>
-      </c>
-      <c r="P4">
-        <v>20</v>
-      </c>
-      <c r="Q4">
-        <f>N4+(O4/60)+(P4/(60*60))</f>
-        <v>33.255555555555553</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5">
-        <v>145</v>
-      </c>
-      <c r="C5">
-        <v>29</v>
-      </c>
-      <c r="D5">
-        <v>20</v>
-      </c>
-      <c r="E5">
-        <f>B5+(C5/60)+(D5/(60*60))</f>
-        <v>145.48888888888888</v>
-      </c>
-      <c r="F5">
-        <v>146</v>
-      </c>
-      <c r="G5">
-        <v>13</v>
-      </c>
-      <c r="H5">
-        <v>4</v>
-      </c>
-      <c r="I5">
-        <f>F5+(G5/60)+(H5/(60*60))</f>
-        <v>146.21777777777777</v>
-      </c>
-      <c r="J5">
-        <v>147</v>
-      </c>
-      <c r="K5">
-        <v>40</v>
-      </c>
-      <c r="L5">
-        <v>30</v>
-      </c>
-      <c r="M5">
-        <f>J5+(K5/60)+(L5/(60*60))</f>
-        <v>147.67499999999998</v>
-      </c>
-      <c r="N5">
-        <v>150</v>
-      </c>
-      <c r="O5">
-        <v>35</v>
-      </c>
-      <c r="P5">
-        <v>4</v>
-      </c>
-      <c r="Q5">
-        <f>N5+(O5/60)+(P5/(60*60))</f>
-        <v>150.58444444444444</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6">
-        <v>38</v>
-      </c>
-      <c r="C6">
-        <v>26</v>
-      </c>
-      <c r="D6">
-        <v>8</v>
-      </c>
-      <c r="E6">
-        <f>B6+(C6/60)+(D6/(60*60))</f>
-        <v>38.435555555555553</v>
-      </c>
-      <c r="F6">
-        <v>39</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>40</v>
-      </c>
-      <c r="I6">
-        <f>F6+(G6/60)+(H6/(60*60))</f>
-        <v>39.011111111111113</v>
-      </c>
-      <c r="J6">
-        <v>40</v>
-      </c>
-      <c r="K6">
-        <v>9</v>
-      </c>
-      <c r="L6">
-        <v>44</v>
-      </c>
-      <c r="M6">
-        <f>J6+(K6/60)+(L6/(60*60))</f>
-        <v>40.162222222222219</v>
-      </c>
-      <c r="N6">
-        <v>42</v>
-      </c>
-      <c r="O6">
-        <v>27</v>
-      </c>
-      <c r="P6">
-        <v>52</v>
-      </c>
-      <c r="Q6">
-        <f>N6+(O6/60)+(P6/(60*60))</f>
-        <v>42.464444444444446</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7">
-        <v>144</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>52</v>
-      </c>
-      <c r="E7">
-        <f>B7+(C7/60)+(D7/(60*60))</f>
-        <v>144.03111111111113</v>
-      </c>
-      <c r="F7">
-        <v>143</v>
-      </c>
-      <c r="G7">
-        <v>18</v>
-      </c>
-      <c r="H7">
-        <v>8</v>
-      </c>
-      <c r="I7">
-        <f>F7+(G7/60)+(H7/(60*60))</f>
-        <v>143.30222222222224</v>
-      </c>
-      <c r="J7">
-        <v>141</v>
-      </c>
-      <c r="K7">
-        <v>50</v>
-      </c>
-      <c r="L7">
-        <v>42</v>
-      </c>
-      <c r="M7">
-        <f>J7+(K7/60)+(L7/(60*60))</f>
-        <v>141.845</v>
-      </c>
-      <c r="N7">
-        <v>138</v>
-      </c>
-      <c r="O7">
-        <v>56</v>
-      </c>
-      <c r="P7">
-        <v>8</v>
-      </c>
-      <c r="Q7">
-        <f>N7+(O7/60)+(P7/(60*60))</f>
-        <v>138.93555555555557</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A9" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A10" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G11" t="s">
-        <v>3</v>
-      </c>
-      <c r="H11" t="s">
-        <v>4</v>
-      </c>
-      <c r="I11" t="s">
-        <v>5</v>
-      </c>
-      <c r="J11" t="s">
-        <v>2</v>
-      </c>
-      <c r="K11" t="s">
-        <v>3</v>
-      </c>
-      <c r="L11" t="s">
-        <v>4</v>
-      </c>
-      <c r="M11" t="s">
-        <v>5</v>
-      </c>
-      <c r="N11" t="s">
-        <v>2</v>
-      </c>
-      <c r="O11" t="s">
-        <v>3</v>
-      </c>
-      <c r="P11" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12">
-        <v>35</v>
-      </c>
-      <c r="C12">
-        <v>27</v>
-      </c>
-      <c r="D12">
-        <v>16</v>
-      </c>
-      <c r="E12">
-        <f>B12+(C12/60)+(D12/(60*60))</f>
-        <v>35.454444444444448</v>
-      </c>
-      <c r="F12">
-        <v>34</v>
-      </c>
-      <c r="G12">
-        <v>52</v>
-      </c>
-      <c r="H12">
-        <v>44</v>
-      </c>
-      <c r="I12">
-        <f>F12+(G12/60)+(H12/(60*60))</f>
-        <v>34.878888888888888</v>
-      </c>
-      <c r="J12">
-        <v>33</v>
-      </c>
-      <c r="K12">
-        <v>43</v>
-      </c>
-      <c r="L12">
-        <v>40</v>
-      </c>
-      <c r="M12">
-        <f>J12+(K12/60)+(L12/(60*60))</f>
-        <v>33.727777777777781</v>
-      </c>
-      <c r="N12">
-        <v>31</v>
-      </c>
-      <c r="O12">
-        <v>25</v>
-      </c>
-      <c r="P12">
-        <v>32</v>
-      </c>
-      <c r="Q12">
-        <f>N12+(O12/60)+(P12/(60*60))</f>
-        <v>31.425555555555558</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13">
-        <v>146</v>
-      </c>
-      <c r="C13">
-        <v>44</v>
-      </c>
-      <c r="D13">
-        <v>30</v>
-      </c>
-      <c r="E13">
-        <f>B13+(C13/60)+(D13/(60*60))</f>
-        <v>146.74166666666665</v>
-      </c>
-      <c r="F13">
-        <v>147</v>
-      </c>
-      <c r="G13">
-        <v>27</v>
-      </c>
-      <c r="H13">
-        <v>12</v>
-      </c>
-      <c r="I13">
-        <f>F13+(G13/60)+(H13/(60*60))</f>
-        <v>147.45333333333332</v>
-      </c>
-      <c r="J13">
-        <v>148</v>
-      </c>
-      <c r="K13">
-        <v>52</v>
-      </c>
-      <c r="L13">
-        <v>34</v>
-      </c>
-      <c r="M13">
-        <f>J13+(K13/60)+(L13/(60*60))</f>
-        <v>148.87611111111113</v>
-      </c>
-      <c r="N13">
-        <v>151</v>
-      </c>
-      <c r="O13">
-        <v>43</v>
-      </c>
-      <c r="P13">
-        <v>2</v>
-      </c>
-      <c r="Q13">
-        <f>N13+(O13/60)+(P13/(60*60))</f>
-        <v>151.71722222222223</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B14">
-        <v>36</v>
-      </c>
-      <c r="C14">
-        <v>36</v>
-      </c>
-      <c r="D14">
-        <v>20</v>
-      </c>
-      <c r="E14">
-        <f>B14+(C14/60)+(D14/(60*60))</f>
-        <v>36.605555555555554</v>
-      </c>
-      <c r="F14">
-        <v>37</v>
-      </c>
-      <c r="G14">
-        <v>10</v>
-      </c>
-      <c r="H14">
-        <v>52</v>
-      </c>
-      <c r="I14">
-        <f>F14+(G14/60)+(H14/(60*60))</f>
-        <v>37.181111111111107</v>
-      </c>
-      <c r="J14">
-        <v>38</v>
-      </c>
-      <c r="K14">
-        <v>19</v>
-      </c>
-      <c r="L14">
-        <v>56</v>
-      </c>
-      <c r="M14">
-        <f>J14+(K14/60)+(L14/(60*60))</f>
-        <v>38.332222222222228</v>
-      </c>
-      <c r="N14">
-        <v>40</v>
-      </c>
-      <c r="O14">
-        <v>38</v>
-      </c>
-      <c r="P14">
-        <v>4</v>
-      </c>
-      <c r="Q14">
-        <f>N14+(O14/60)+(P14/(60*60))</f>
-        <v>40.634444444444441</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
-        <v>65</v>
-      </c>
-      <c r="B15">
-        <v>145</v>
-      </c>
-      <c r="C15">
-        <v>19</v>
-      </c>
-      <c r="D15">
-        <v>6</v>
-      </c>
-      <c r="E15">
-        <f>B15+(C15/60)+(D15/(60*60))</f>
-        <v>145.31833333333333</v>
-      </c>
-      <c r="F15">
-        <v>144</v>
-      </c>
-      <c r="G15">
-        <v>36</v>
-      </c>
-      <c r="H15">
-        <v>24</v>
-      </c>
-      <c r="I15">
-        <f>F15+(G15/60)+(H15/(60*60))</f>
-        <v>144.60666666666665</v>
-      </c>
-      <c r="J15">
-        <v>143</v>
-      </c>
-      <c r="K15">
-        <v>11</v>
-      </c>
-      <c r="L15">
-        <v>22</v>
-      </c>
-      <c r="M15">
-        <f>J15+(K15/60)+(L15/(60*60))</f>
-        <v>143.18944444444446</v>
-      </c>
-      <c r="N15">
-        <v>140</v>
-      </c>
-      <c r="O15">
-        <v>20</v>
-      </c>
-      <c r="P15">
-        <v>34</v>
-      </c>
-      <c r="Q15">
-        <f>N15+(O15/60)+(P15/(60*60))</f>
-        <v>140.3427777777778</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
0.0.b19 Adjust TRIM Gui aesthetics
Created a little more spacing in the button on the trim gui. Looks a little better than what it was.
</commit_message>
<xml_diff>
--- a/Roadmap.xlsx
+++ b/Roadmap.xlsx
@@ -24619,8 +24619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="B20" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -24828,7 +24828,7 @@
       <c r="B15" t="s">
         <v>591</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="24" t="s">
         <v>536</v>
       </c>
       <c r="E15" s="24" t="s">
@@ -24861,7 +24861,7 @@
       <c r="B18" t="s">
         <v>594</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="24" t="s">
         <v>750</v>
       </c>
     </row>
@@ -24869,7 +24869,7 @@
       <c r="B19" t="s">
         <v>595</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="24" t="s">
         <v>558</v>
       </c>
     </row>
@@ -24877,7 +24877,7 @@
       <c r="B20" t="s">
         <v>596</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="24" t="s">
         <v>559</v>
       </c>
     </row>
@@ -24885,7 +24885,7 @@
       <c r="B21" t="s">
         <v>597</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="24" t="s">
         <v>560</v>
       </c>
     </row>
@@ -24896,7 +24896,7 @@
       <c r="D22" t="s">
         <v>538</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="24" t="s">
         <v>561</v>
       </c>
     </row>

</xml_diff>